<commit_message>
Agrega renglón Ganancia Acumulada en la hojda Ganancia_total_90_dicc1
</commit_message>
<xml_diff>
--- a/experimentos/compara_experimentos_articulo.xlsx
+++ b/experimentos/compara_experimentos_articulo.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="53">
   <si>
     <t>Periodo Prueba</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>Máxima pérdida</t>
+  </si>
+  <si>
+    <t>Ganancia Acumulada</t>
   </si>
 </sst>
 </file>
@@ -192,11 +195,12 @@
     <numFmt numFmtId="168" formatCode="0.00"/>
     <numFmt numFmtId="169" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -215,12 +219,6 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -286,7 +284,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -327,14 +325,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="70.734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="18.469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.3112244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.2551020408163"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="12.3112244897959"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="13.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="71.9234693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3367346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="18.6836734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5255102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="12.5255102040816"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="13.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1740,14 +1738,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="70.734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="18.469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.3112244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.2551020408163"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="12.3112244897959"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="13.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="71.9234693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3367346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="18.6836734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5255102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="12.5255102040816"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="13.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3132,7 +3130,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3145,22 +3143,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
+      <selection pane="topLeft" activeCell="F36" activeCellId="0" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="70.734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="18.469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.3112244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.2551020408163"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="12.3112244897959"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="13.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="71.9234693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3367346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="18.6836734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5255102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="12.5255102040816"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="13.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4100,222 +4098,259 @@
     </row>
     <row r="36" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="5" t="n">
+        <f aca="false">SUM(B2:B31)</f>
+        <v>71525.5387355434</v>
+      </c>
+      <c r="C36" s="5" t="n">
+        <f aca="false">SUM(C2:C31)</f>
+        <v>48603.2789436188</v>
+      </c>
+      <c r="D36" s="5" t="n">
+        <f aca="false">SUM(D2:D31)</f>
+        <v>66445.0778375695</v>
+      </c>
+      <c r="E36" s="5" t="n">
+        <f aca="false">SUM(E2:E31)</f>
+        <v>29848.8984266699</v>
+      </c>
+      <c r="F36" s="5" t="n">
+        <f aca="false">SUM(F2:F31)</f>
+        <v>23772.9861160162</v>
+      </c>
+      <c r="G36" s="5" t="n">
+        <f aca="false">SUM(G2:G31)</f>
+        <v>28382.1906925601</v>
+      </c>
+      <c r="H36" s="5" t="n">
+        <f aca="false">SUM(H2:H31)</f>
+        <v>44251.0843369546</v>
+      </c>
+      <c r="I36" s="5" t="n">
+        <f aca="false">SUM(I2:I31)</f>
+        <v>18149.682509695</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="5" t="n">
+      <c r="B37" s="5" t="n">
         <f aca="false">AVERAGE(B2:B31)</f>
         <v>2384.18462451811</v>
       </c>
-      <c r="C36" s="5" t="n">
+      <c r="C37" s="5" t="n">
         <f aca="false">AVERAGE(C2:C31)</f>
         <v>1620.10929812063</v>
       </c>
-      <c r="D36" s="5" t="n">
+      <c r="D37" s="5" t="n">
         <f aca="false">AVERAGE(D2:D31)</f>
         <v>2214.83592791898</v>
       </c>
-      <c r="E36" s="5" t="n">
+      <c r="E37" s="5" t="n">
         <f aca="false">AVERAGE(E2:E31)</f>
         <v>994.963280889001</v>
       </c>
-      <c r="F36" s="5" t="n">
+      <c r="F37" s="5" t="n">
         <f aca="false">AVERAGE(F2:F31)</f>
         <v>792.432870533874</v>
       </c>
-      <c r="G36" s="5" t="n">
+      <c r="G37" s="5" t="n">
         <f aca="false">AVERAGE(G2:G31)</f>
         <v>946.073023085334</v>
       </c>
-      <c r="H36" s="5" t="n">
+      <c r="H37" s="5" t="n">
         <f aca="false">AVERAGE(H2:H31)</f>
         <v>1475.03614456516</v>
       </c>
-      <c r="I36" s="5" t="n">
+      <c r="I37" s="5" t="n">
         <f aca="false">AVERAGE(I2:I31)</f>
         <v>604.989416989836</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+    <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="5" t="n">
+      <c r="B38" s="5" t="n">
         <f aca="false">STDEV(B2:B31)</f>
         <v>6656.27000888295</v>
       </c>
-      <c r="C37" s="5" t="n">
+      <c r="C38" s="5" t="n">
         <f aca="false">STDEV(C2:C31)</f>
         <v>6614.6617668422</v>
       </c>
-      <c r="D37" s="5" t="n">
+      <c r="D38" s="5" t="n">
         <f aca="false">STDEV(D2:D31)</f>
         <v>6996.64380426849</v>
       </c>
-      <c r="E37" s="5" t="n">
+      <c r="E38" s="5" t="n">
         <f aca="false">STDEV(E2:E31)</f>
         <v>6717.04596795076</v>
       </c>
-      <c r="F37" s="5" t="n">
+      <c r="F38" s="5" t="n">
         <f aca="false">STDEV(F2:F31)</f>
         <v>7475.2731819457</v>
       </c>
-      <c r="G37" s="5" t="n">
+      <c r="G38" s="5" t="n">
         <f aca="false">STDEV(G2:G31)</f>
         <v>8228.07887606131</v>
       </c>
-      <c r="H37" s="5" t="n">
+      <c r="H38" s="5" t="n">
         <f aca="false">STDEV(H2:H31)</f>
         <v>7867.32637550916</v>
       </c>
-      <c r="I37" s="5" t="n">
+      <c r="I38" s="5" t="n">
         <f aca="false">STDEV(I2:I31)</f>
         <v>8802.12418065692</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+    <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="0" t="n">
+      <c r="B39" s="0" t="n">
         <f aca="false">COUNTIF(B2:B31,"&gt;0")</f>
         <v>20</v>
       </c>
-      <c r="C38" s="0" t="n">
+      <c r="C39" s="0" t="n">
         <f aca="false">COUNTIF(C2:C31,"&gt;0")</f>
         <v>21</v>
       </c>
-      <c r="D38" s="0" t="n">
+      <c r="D39" s="0" t="n">
         <f aca="false">COUNTIF(D2:D31,"&gt;0")</f>
         <v>19</v>
       </c>
-      <c r="E38" s="0" t="n">
+      <c r="E39" s="0" t="n">
         <f aca="false">COUNTIF(E2:E31,"&gt;0")</f>
         <v>19</v>
       </c>
-      <c r="F38" s="0" t="n">
+      <c r="F39" s="0" t="n">
         <f aca="false">COUNTIF(F2:F31,"&gt;0")</f>
         <v>19</v>
       </c>
-      <c r="G38" s="0" t="n">
+      <c r="G39" s="0" t="n">
         <f aca="false">COUNTIF(G2:G31,"&gt;0")</f>
         <v>20</v>
       </c>
-      <c r="H38" s="0" t="n">
+      <c r="H39" s="0" t="n">
         <f aca="false">COUNTIF(H2:H31,"&gt;0")</f>
         <v>20</v>
       </c>
-      <c r="I38" s="0" t="n">
+      <c r="I39" s="0" t="n">
         <f aca="false">COUNTIF(I2:I31,"&gt;0")</f>
         <v>19</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+    <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="B39" s="0" t="n">
+      <c r="B40" s="0" t="n">
         <f aca="false">COUNTIF(B2:B31,"&lt;=0")</f>
         <v>10</v>
       </c>
-      <c r="C39" s="0" t="n">
+      <c r="C40" s="0" t="n">
         <f aca="false">COUNTIF(C2:C31,"&lt;=0")</f>
         <v>9</v>
       </c>
-      <c r="D39" s="0" t="n">
+      <c r="D40" s="0" t="n">
         <f aca="false">COUNTIF(D2:D31,"&lt;=0")</f>
         <v>11</v>
       </c>
-      <c r="E39" s="0" t="n">
+      <c r="E40" s="0" t="n">
         <f aca="false">COUNTIF(E2:E31,"&lt;=0")</f>
         <v>11</v>
       </c>
-      <c r="F39" s="0" t="n">
+      <c r="F40" s="0" t="n">
         <f aca="false">COUNTIF(F2:F31,"&lt;=0")</f>
         <v>11</v>
       </c>
-      <c r="G39" s="0" t="n">
+      <c r="G40" s="0" t="n">
         <f aca="false">COUNTIF(G2:G31,"&lt;=0")</f>
         <v>10</v>
       </c>
-      <c r="H39" s="0" t="n">
+      <c r="H40" s="0" t="n">
         <f aca="false">COUNTIF(H2:H31,"&lt;=0")</f>
         <v>10</v>
       </c>
-      <c r="I39" s="0" t="n">
+      <c r="I40" s="0" t="n">
         <f aca="false">COUNTIF(I2:I31,"&lt;=0")</f>
         <v>11</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+    <row r="41" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="B40" s="5" t="n">
+      <c r="B41" s="5" t="n">
         <f aca="false">MAX(B2:B31)</f>
         <v>17247.1701471001</v>
       </c>
-      <c r="C40" s="5" t="n">
+      <c r="C41" s="5" t="n">
         <f aca="false">MAX(C2:C31)</f>
         <v>12764.2969688301</v>
       </c>
-      <c r="D40" s="5" t="n">
+      <c r="D41" s="5" t="n">
         <f aca="false">MAX(D2:D31)</f>
         <v>16400.7522481838</v>
       </c>
-      <c r="E40" s="5" t="n">
+      <c r="E41" s="5" t="n">
         <f aca="false">MAX(E2:E31)</f>
         <v>13657.7017121613</v>
       </c>
-      <c r="F40" s="5" t="n">
+      <c r="F41" s="5" t="n">
         <f aca="false">MAX(F2:F31)</f>
         <v>15012.2416079563</v>
       </c>
-      <c r="G40" s="5" t="n">
+      <c r="G41" s="5" t="n">
         <f aca="false">MAX(G2:G31)</f>
         <v>19151.8633369488</v>
       </c>
-      <c r="H40" s="5" t="n">
+      <c r="H41" s="5" t="n">
         <f aca="false">MAX(H2:H31)</f>
         <v>15338.9847221538</v>
       </c>
-      <c r="I40" s="5" t="n">
+      <c r="I41" s="5" t="n">
         <f aca="false">MAX(I2:I31)</f>
         <v>10359.8286045001</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+    <row r="42" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="5" t="n">
+      <c r="B42" s="5" t="n">
         <f aca="false">MIN(B2:B31)</f>
         <v>-14512.5087876937</v>
       </c>
-      <c r="C41" s="5" t="n">
+      <c r="C42" s="5" t="n">
         <f aca="false">MIN(C2:C31)</f>
         <v>-13311.8810443912</v>
       </c>
-      <c r="D41" s="5" t="n">
+      <c r="D42" s="5" t="n">
         <f aca="false">MIN(D2:D31)</f>
         <v>-11183.9199377187</v>
       </c>
-      <c r="E41" s="5" t="n">
+      <c r="E42" s="5" t="n">
         <f aca="false">MIN(E2:E31)</f>
         <v>-13249.9806496087</v>
       </c>
-      <c r="F41" s="5" t="n">
+      <c r="F42" s="5" t="n">
         <f aca="false">MIN(F2:F31)</f>
         <v>-17590.5677236762</v>
       </c>
-      <c r="G41" s="5" t="n">
+      <c r="G42" s="5" t="n">
         <f aca="false">MIN(G2:G31)</f>
         <v>-20961.8907815036</v>
       </c>
-      <c r="H41" s="5" t="n">
+      <c r="H42" s="5" t="n">
         <f aca="false">MIN(H2:H31)</f>
         <v>-21472.5499429262</v>
       </c>
-      <c r="I41" s="5" t="n">
+      <c r="I42" s="5" t="n">
         <f aca="false">MIN(I2:I31)</f>
         <v>-33896.8352725949</v>
       </c>
@@ -4323,7 +4358,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Agrega comparación sin crisis de 2008
</commit_message>
<xml_diff>
--- a/experimentos/compara_experimentos_articulo.xlsx
+++ b/experimentos/compara_experimentos_articulo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Exceso_sobre_BH_NORMAL_90_dicc1_PENALIZA" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="55">
   <si>
     <t>Periodo Prueba</t>
   </si>
@@ -150,22 +150,7 @@
     <t>Promedio por 100 mil unidades de inversión</t>
   </si>
   <si>
-    <t>Promedio (Anualizado – multiplicado por 4)</t>
-  </si>
-  <si>
-    <t>Promedio (Anualizado – por cada 100 mil pesos invertidos)</t>
-  </si>
-  <si>
-    <t>Desviación Estándar (Riesgo, anualizado – multiplicado por sqrt(4))</t>
-  </si>
-  <si>
-    <t>Desviación Estándar (Riesgo, anualizado – por cada 100 mil pesos)</t>
-  </si>
-  <si>
-    <t>Sharpe Ratio (Anualizado)</t>
-  </si>
-  <si>
-    <t>Sharpe Ratio (Anualizado – por cada 100 mil pesos)</t>
+    <t>Desviación estándar</t>
   </si>
   <si>
     <t>Número de casos en los que se gana</t>
@@ -180,20 +165,40 @@
     <t>Máxima pérdida</t>
   </si>
   <si>
-    <t>Ganancia Acumulada</t>
+    <t>Promedio sin crisis 2008</t>
+  </si>
+  <si>
+    <t>Promedio sin crisis 2008 por 100 mil unidades de inversión</t>
+  </si>
+  <si>
+    <t>Desviación estándar sin crisis 2008</t>
+  </si>
+  <si>
+    <t>Número de casos en los que se gana sin crisis 2008</t>
+  </si>
+  <si>
+    <t>Número de casos en los que se pierde sin crisis 2008</t>
+  </si>
+  <si>
+    <t>Máxima ganancia sin crisis 2008</t>
+  </si>
+  <si>
+    <t>Máxima pérdida sin crisis 2008</t>
+  </si>
+  <si>
+    <t>Desviación Estándar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
     <numFmt numFmtId="167" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
-    <numFmt numFmtId="168" formatCode="0.00"/>
-    <numFmt numFmtId="169" formatCode="0.00E+00"/>
+    <numFmt numFmtId="168" formatCode="0.00E+00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -267,7 +272,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -280,11 +285,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -293,10 +298,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -317,22 +318,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="71.9234693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3367346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="18.6836734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5255102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="12.5255102040816"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="13.6071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.75"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="73.1122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.7448979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.6887755102041"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="12.7448979591837"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="13.7142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.85714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1268,47 +1269,70 @@
       <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="3"/>
+      <c r="B35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="3" t="n">
+      <c r="B36" s="4" t="n">
         <f aca="false">AVERAGE(B2:B31)</f>
         <v>0.00372447265282125</v>
       </c>
-      <c r="C36" s="3" t="n">
+      <c r="C36" s="4" t="n">
         <f aca="false">AVERAGE(C2:C31)</f>
         <v>-0.00391628060760466</v>
       </c>
-      <c r="D36" s="3" t="n">
+      <c r="D36" s="4" t="n">
         <f aca="false">AVERAGE(D2:D31)</f>
         <v>0.00203098569037882</v>
       </c>
-      <c r="E36" s="3" t="n">
+      <c r="E36" s="4" t="n">
         <f aca="false">AVERAGE(E2:E31)</f>
         <v>-0.010167740779921</v>
       </c>
-      <c r="F36" s="3" t="n">
+      <c r="F36" s="4" t="n">
         <f aca="false">AVERAGE(F2:F31)</f>
         <v>-0.0121930448834722</v>
       </c>
-      <c r="G36" s="3" t="n">
+      <c r="G36" s="4" t="n">
         <f aca="false">AVERAGE(G2:G31)</f>
         <v>-0.0106566433579576</v>
       </c>
-      <c r="H36" s="3" t="n">
+      <c r="H36" s="4" t="n">
         <f aca="false">AVERAGE(H2:H31)</f>
         <v>-0.00536701214315941</v>
       </c>
-      <c r="I36" s="3" t="n">
+      <c r="I36" s="4" t="n">
         <f aca="false">AVERAGE(I2:I31)</f>
         <v>-0.0140674794189126</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="5" t="n">
@@ -1345,372 +1369,446 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="3" t="n">
-        <f aca="false">AVERAGE(B2:B31)*4</f>
-        <v>0.014897890611285</v>
-      </c>
-      <c r="C38" s="3" t="n">
-        <f aca="false">AVERAGE(C2:C31)*4</f>
-        <v>-0.0156651224304187</v>
-      </c>
-      <c r="D38" s="3" t="n">
-        <f aca="false">AVERAGE(D2:D31)*4</f>
-        <v>0.00812394276151528</v>
-      </c>
-      <c r="E38" s="3" t="n">
-        <f aca="false">AVERAGE(E2:E31)*4</f>
-        <v>-0.0406709631196838</v>
-      </c>
-      <c r="F38" s="3" t="n">
-        <f aca="false">AVERAGE(F2:F31)*4</f>
-        <v>-0.0487721795338889</v>
-      </c>
-      <c r="G38" s="3" t="n">
-        <f aca="false">AVERAGE(G2:G31)*4</f>
-        <v>-0.0426265734318305</v>
-      </c>
-      <c r="H38" s="3" t="n">
-        <f aca="false">AVERAGE(H2:H31)*4</f>
-        <v>-0.0214680485726376</v>
-      </c>
-      <c r="I38" s="3" t="n">
-        <f aca="false">AVERAGE(I2:I31)*4</f>
-        <v>-0.0562699176756504</v>
+      <c r="B38" s="4" t="n">
+        <f aca="false">STDEV(B2:B31)</f>
+        <v>0.0710680418327085</v>
+      </c>
+      <c r="C38" s="4" t="n">
+        <f aca="false">STDEV(C2:C31)</f>
+        <v>0.0564452151984446</v>
+      </c>
+      <c r="D38" s="4" t="n">
+        <f aca="false">STDEV(D2:D31)</f>
+        <v>0.0597861371142287</v>
+      </c>
+      <c r="E38" s="4" t="n">
+        <f aca="false">STDEV(E2:E31)</f>
+        <v>0.0538802574663418</v>
+      </c>
+      <c r="F38" s="4" t="n">
+        <f aca="false">STDEV(F2:F31)</f>
+        <v>0.0453399118991043</v>
+      </c>
+      <c r="G38" s="4" t="n">
+        <f aca="false">STDEV(G2:G31)</f>
+        <v>0.0461630217065584</v>
+      </c>
+      <c r="H38" s="4" t="n">
+        <f aca="false">STDEV(H2:H31)</f>
+        <v>0.0319772866643594</v>
+      </c>
+      <c r="I38" s="4" t="n">
+        <f aca="false">STDEV(I2:I31)</f>
+        <v>0.0317401523043012</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="6" t="n">
-        <f aca="false">B38*100000</f>
-        <v>1489.7890611285</v>
-      </c>
-      <c r="C39" s="6" t="n">
-        <f aca="false">C38*100000</f>
-        <v>-1566.51224304187</v>
-      </c>
-      <c r="D39" s="6" t="n">
-        <f aca="false">D38*100000</f>
-        <v>812.394276151528</v>
-      </c>
-      <c r="E39" s="6" t="n">
-        <f aca="false">E38*100000</f>
-        <v>-4067.09631196838</v>
-      </c>
-      <c r="F39" s="6" t="n">
-        <f aca="false">F38*100000</f>
-        <v>-4877.21795338889</v>
-      </c>
-      <c r="G39" s="6" t="n">
-        <f aca="false">G38*100000</f>
-        <v>-4262.65734318305</v>
-      </c>
-      <c r="H39" s="6" t="n">
-        <f aca="false">H38*100000</f>
-        <v>-2146.80485726376</v>
-      </c>
-      <c r="I39" s="6" t="n">
-        <f aca="false">I38*100000</f>
-        <v>-5626.99176756504</v>
+      <c r="B39" s="0" t="n">
+        <f aca="false">COUNTIF(B2:B31,"&gt;0")</f>
+        <v>11</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <f aca="false">COUNTIF(C2:C31,"&gt;0")</f>
+        <v>14</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <f aca="false">COUNTIF(D2:D31,"&gt;0")</f>
+        <v>10</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <f aca="false">COUNTIF(E2:E31,"&gt;0")</f>
+        <v>13</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <f aca="false">COUNTIF(F2:F31,"&gt;0")</f>
+        <v>11</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <f aca="false">COUNTIF(G2:G31,"&gt;0")</f>
+        <v>10</v>
+      </c>
+      <c r="H39" s="0" t="n">
+        <f aca="false">COUNTIF(H2:H31,"&gt;0")</f>
+        <v>12</v>
+      </c>
+      <c r="I39" s="0" t="n">
+        <f aca="false">COUNTIF(I2:I31,"&gt;0")</f>
+        <v>8</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="2" t="n">
-        <f aca="false">STDEV(B2:B31)*SQRT(4)</f>
-        <v>0.142136083665417</v>
-      </c>
-      <c r="C40" s="2" t="n">
-        <f aca="false">STDEV(C2:C31)*SQRT(4)</f>
-        <v>0.112890430396889</v>
-      </c>
-      <c r="D40" s="2" t="n">
-        <f aca="false">STDEV(D2:D31)*SQRT(4)</f>
-        <v>0.119572274228457</v>
-      </c>
-      <c r="E40" s="2" t="n">
-        <f aca="false">STDEV(E2:E31)*SQRT(4)</f>
-        <v>0.107760514932683</v>
-      </c>
-      <c r="F40" s="2" t="n">
-        <f aca="false">STDEV(F2:F31)*SQRT(4)</f>
-        <v>0.0906798237982084</v>
-      </c>
-      <c r="G40" s="2" t="n">
-        <f aca="false">STDEV(G2:G31)*SQRT(4)</f>
-        <v>0.0923260434131167</v>
-      </c>
-      <c r="H40" s="2" t="n">
-        <f aca="false">STDEV(H2:H31)*SQRT(4)</f>
-        <v>0.0639545733287186</v>
-      </c>
-      <c r="I40" s="2" t="n">
-        <f aca="false">STDEV(I2:I31)*SQRT(4)</f>
-        <v>0.0634803046086024</v>
+      <c r="B40" s="0" t="n">
+        <f aca="false">COUNTIF(B2:B31,"&lt;=0")</f>
+        <v>19</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <f aca="false">COUNTIF(C2:C31,"&lt;=0")</f>
+        <v>16</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <f aca="false">COUNTIF(D2:D31,"&lt;=0")</f>
+        <v>20</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <f aca="false">COUNTIF(E2:E31,"&lt;=0")</f>
+        <v>17</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <f aca="false">COUNTIF(F2:F31,"&lt;=0")</f>
+        <v>19</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <f aca="false">COUNTIF(G2:G31,"&lt;=0")</f>
+        <v>20</v>
+      </c>
+      <c r="H40" s="0" t="n">
+        <f aca="false">COUNTIF(H2:H31,"&lt;=0")</f>
+        <v>18</v>
+      </c>
+      <c r="I40" s="0" t="n">
+        <f aca="false">COUNTIF(I2:I31,"&lt;=0")</f>
+        <v>22</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="6" t="n">
-        <f aca="false">B40*100000</f>
-        <v>14213.6083665417</v>
-      </c>
-      <c r="C41" s="6" t="n">
-        <f aca="false">C40*100000</f>
-        <v>11289.0430396889</v>
-      </c>
-      <c r="D41" s="6" t="n">
-        <f aca="false">D40*100000</f>
-        <v>11957.2274228457</v>
-      </c>
-      <c r="E41" s="6" t="n">
-        <f aca="false">E40*100000</f>
-        <v>10776.0514932683</v>
-      </c>
-      <c r="F41" s="6" t="n">
-        <f aca="false">F40*100000</f>
-        <v>9067.98237982084</v>
-      </c>
-      <c r="G41" s="6" t="n">
-        <f aca="false">G40*100000</f>
-        <v>9232.60434131167</v>
-      </c>
-      <c r="H41" s="6" t="n">
-        <f aca="false">H40*100000</f>
-        <v>6395.45733287186</v>
-      </c>
-      <c r="I41" s="6" t="n">
-        <f aca="false">I40*100000</f>
-        <v>6348.03046086024</v>
+      <c r="B41" s="4" t="n">
+        <f aca="false">MAX(B2:B31)</f>
+        <v>0.3463976006</v>
+      </c>
+      <c r="C41" s="4" t="n">
+        <f aca="false">MAX(C2:C31)</f>
+        <v>0.221661110373976</v>
+      </c>
+      <c r="D41" s="4" t="n">
+        <f aca="false">MAX(D2:D31)</f>
+        <v>0.297155670571326</v>
+      </c>
+      <c r="E41" s="4" t="n">
+        <f aca="false">MAX(E2:E31)</f>
+        <v>0.203655817993814</v>
+      </c>
+      <c r="F41" s="4" t="n">
+        <f aca="false">MAX(F2:F31)</f>
+        <v>0.156874580187626</v>
+      </c>
+      <c r="G41" s="4" t="n">
+        <f aca="false">MAX(G2:G31)</f>
+        <v>0.123161349609351</v>
+      </c>
+      <c r="H41" s="4" t="n">
+        <f aca="false">MAX(H2:H31)</f>
+        <v>0.118054757995126</v>
+      </c>
+      <c r="I41" s="4" t="n">
+        <f aca="false">MAX(I2:I31)</f>
+        <v>0.0604585318305874</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B42" s="6" t="n">
-        <f aca="false">B38/B40</f>
-        <v>0.10481427535568</v>
-      </c>
-      <c r="C42" s="6" t="n">
-        <f aca="false">C38/C40</f>
-        <v>-0.138763953466602</v>
-      </c>
-      <c r="D42" s="6" t="n">
-        <f aca="false">D38/D40</f>
-        <v>0.0679416931218813</v>
-      </c>
-      <c r="E42" s="6" t="n">
-        <f aca="false">E38/E40</f>
-        <v>-0.377419903246476</v>
-      </c>
-      <c r="F42" s="6" t="n">
-        <f aca="false">F38/F40</f>
-        <v>-0.537850400353916</v>
-      </c>
-      <c r="G42" s="6" t="n">
-        <f aca="false">G38/G40</f>
-        <v>-0.461696091980202</v>
-      </c>
-      <c r="H42" s="6" t="n">
-        <f aca="false">H38/H40</f>
-        <v>-0.33567651936781</v>
-      </c>
-      <c r="I42" s="6" t="n">
-        <f aca="false">I38/I40</f>
-        <v>-0.886415369658216</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" s="6" t="n">
-        <f aca="false">B42*100000</f>
-        <v>10481.427535568</v>
-      </c>
-      <c r="C43" s="6" t="n">
-        <f aca="false">C42*100000</f>
-        <v>-13876.3953466602</v>
-      </c>
-      <c r="D43" s="6" t="n">
-        <f aca="false">D42*100000</f>
-        <v>6794.16931218813</v>
-      </c>
-      <c r="E43" s="6" t="n">
-        <f aca="false">E42*100000</f>
-        <v>-37741.9903246476</v>
-      </c>
-      <c r="F43" s="6" t="n">
-        <f aca="false">F42*100000</f>
-        <v>-53785.0400353916</v>
-      </c>
-      <c r="G43" s="6" t="n">
-        <f aca="false">G42*100000</f>
-        <v>-46169.6091980202</v>
-      </c>
-      <c r="H43" s="6" t="n">
-        <f aca="false">H42*100000</f>
-        <v>-33567.651936781</v>
-      </c>
-      <c r="I43" s="6" t="n">
-        <f aca="false">I42*100000</f>
-        <v>-88641.5369658216</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44" s="0" t="n">
-        <f aca="false">COUNTIF(B2:B31,"&gt;0")</f>
-        <v>11</v>
-      </c>
-      <c r="C44" s="0" t="n">
-        <f aca="false">COUNTIF(C2:C31,"&gt;0")</f>
-        <v>14</v>
-      </c>
-      <c r="D44" s="0" t="n">
-        <f aca="false">COUNTIF(D2:D31,"&gt;0")</f>
-        <v>10</v>
-      </c>
-      <c r="E44" s="0" t="n">
-        <f aca="false">COUNTIF(E2:E31,"&gt;0")</f>
-        <v>13</v>
-      </c>
-      <c r="F44" s="0" t="n">
-        <f aca="false">COUNTIF(F2:F31,"&gt;0")</f>
-        <v>11</v>
-      </c>
-      <c r="G44" s="0" t="n">
-        <f aca="false">COUNTIF(G2:G31,"&gt;0")</f>
-        <v>10</v>
-      </c>
-      <c r="H44" s="0" t="n">
-        <f aca="false">COUNTIF(H2:H31,"&gt;0")</f>
-        <v>12</v>
-      </c>
-      <c r="I44" s="0" t="n">
-        <f aca="false">COUNTIF(I2:I31,"&gt;0")</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" s="0" t="n">
-        <f aca="false">COUNTIF(B2:B31,"&lt;=0")</f>
-        <v>19</v>
-      </c>
-      <c r="C45" s="0" t="n">
-        <f aca="false">COUNTIF(C2:C31,"&lt;=0")</f>
-        <v>16</v>
-      </c>
-      <c r="D45" s="0" t="n">
-        <f aca="false">COUNTIF(D2:D31,"&lt;=0")</f>
-        <v>20</v>
-      </c>
-      <c r="E45" s="0" t="n">
-        <f aca="false">COUNTIF(E2:E31,"&lt;=0")</f>
-        <v>17</v>
-      </c>
-      <c r="F45" s="0" t="n">
-        <f aca="false">COUNTIF(F2:F31,"&lt;=0")</f>
-        <v>19</v>
-      </c>
-      <c r="G45" s="0" t="n">
-        <f aca="false">COUNTIF(G2:G31,"&lt;=0")</f>
-        <v>20</v>
-      </c>
-      <c r="H45" s="0" t="n">
-        <f aca="false">COUNTIF(H2:H31,"&lt;=0")</f>
-        <v>18</v>
-      </c>
-      <c r="I45" s="0" t="n">
-        <f aca="false">COUNTIF(I2:I31,"&lt;=0")</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46" s="3" t="n">
-        <f aca="false">MAX(B2:B31)</f>
-        <v>0.3463976006</v>
-      </c>
-      <c r="C46" s="3" t="n">
-        <f aca="false">MAX(C2:C31)</f>
-        <v>0.221661110373976</v>
-      </c>
-      <c r="D46" s="3" t="n">
-        <f aca="false">MAX(D2:D31)</f>
-        <v>0.297155670571326</v>
-      </c>
-      <c r="E46" s="3" t="n">
-        <f aca="false">MAX(E2:E31)</f>
-        <v>0.203655817993814</v>
-      </c>
-      <c r="F46" s="3" t="n">
-        <f aca="false">MAX(F2:F31)</f>
-        <v>0.156874580187626</v>
-      </c>
-      <c r="G46" s="3" t="n">
-        <f aca="false">MAX(G2:G31)</f>
-        <v>0.123161349609351</v>
-      </c>
-      <c r="H46" s="3" t="n">
-        <f aca="false">MAX(H2:H31)</f>
-        <v>0.118054757995126</v>
-      </c>
-      <c r="I46" s="3" t="n">
-        <f aca="false">MAX(I2:I31)</f>
-        <v>0.0604585318305874</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B47" s="3" t="n">
+      <c r="B42" s="4" t="n">
         <f aca="false">MIN(B2:B31)</f>
         <v>-0.1123016711</v>
       </c>
-      <c r="C47" s="3" t="n">
+      <c r="C42" s="4" t="n">
         <f aca="false">MIN(C2:C31)</f>
         <v>-0.129376794331987</v>
       </c>
-      <c r="D47" s="3" t="n">
+      <c r="D42" s="4" t="n">
         <f aca="false">MIN(D2:D31)</f>
         <v>-0.0386054491312377</v>
       </c>
-      <c r="E47" s="3" t="n">
+      <c r="E42" s="4" t="n">
         <f aca="false">MIN(E2:E31)</f>
         <v>-0.114673144447425</v>
       </c>
-      <c r="F47" s="3" t="n">
+      <c r="F42" s="4" t="n">
         <f aca="false">MIN(F2:F31)</f>
         <v>-0.128729019240375</v>
       </c>
-      <c r="G47" s="3" t="n">
+      <c r="G42" s="4" t="n">
         <f aca="false">MIN(G2:G31)</f>
         <v>-0.0943216034791614</v>
       </c>
-      <c r="H47" s="3" t="n">
+      <c r="H42" s="4" t="n">
         <f aca="false">MIN(H2:H31)</f>
         <v>-0.0648045595957615</v>
       </c>
-      <c r="I47" s="3" t="n">
+      <c r="I42" s="4" t="n">
         <f aca="false">MIN(I2:I31)</f>
+        <v>-0.0833472266552495</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" s="4" t="n">
+        <f aca="false">AVERAGE(B4:B31)</f>
+        <v>-0.0112852026898344</v>
+      </c>
+      <c r="C43" s="4" t="n">
+        <f aca="false">AVERAGE(C4:C31)</f>
+        <v>-0.01294520102486</v>
+      </c>
+      <c r="D43" s="4" t="n">
+        <f aca="false">AVERAGE(D4:D31)</f>
+        <v>-0.0106308799948825</v>
+      </c>
+      <c r="E43" s="4" t="n">
+        <f aca="false">AVERAGE(E4:E31)</f>
+        <v>-0.0194416852726466</v>
+      </c>
+      <c r="F43" s="4" t="n">
+        <f aca="false">AVERAGE(F4:F31)</f>
+        <v>-0.0187647195060502</v>
+      </c>
+      <c r="G43" s="4" t="n">
+        <f aca="false">AVERAGE(G4:G31)</f>
+        <v>-0.0156799600878627</v>
+      </c>
+      <c r="H43" s="4" t="n">
+        <f aca="false">AVERAGE(H4:H31)</f>
+        <v>-0.0117746128553489</v>
+      </c>
+      <c r="I43" s="4" t="n">
+        <f aca="false">AVERAGE(I4:I31)</f>
+        <v>-0.013848781134268</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" s="5" t="n">
+        <f aca="false">B43*100000</f>
+        <v>-1128.52026898344</v>
+      </c>
+      <c r="C44" s="5" t="n">
+        <f aca="false">C43*100000</f>
+        <v>-1294.520102486</v>
+      </c>
+      <c r="D44" s="5" t="n">
+        <f aca="false">D43*100000</f>
+        <v>-1063.08799948825</v>
+      </c>
+      <c r="E44" s="5" t="n">
+        <f aca="false">E43*100000</f>
+        <v>-1944.16852726466</v>
+      </c>
+      <c r="F44" s="5" t="n">
+        <f aca="false">F43*100000</f>
+        <v>-1876.47195060502</v>
+      </c>
+      <c r="G44" s="5" t="n">
+        <f aca="false">G43*100000</f>
+        <v>-1567.99600878627</v>
+      </c>
+      <c r="H44" s="5" t="n">
+        <f aca="false">H43*100000</f>
+        <v>-1177.46128553489</v>
+      </c>
+      <c r="I44" s="5" t="n">
+        <f aca="false">I43*100000</f>
+        <v>-1384.8781134268</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="4" t="n">
+        <f aca="false">STDEV(B4:B31)</f>
+        <v>0.0248811339248954</v>
+      </c>
+      <c r="C45" s="4" t="n">
+        <f aca="false">STDEV(C4:C31)</f>
+        <v>0.0377547868219428</v>
+      </c>
+      <c r="D45" s="4" t="n">
+        <f aca="false">STDEV(D4:D31)</f>
+        <v>0.0177849362099375</v>
+      </c>
+      <c r="E45" s="4" t="n">
+        <f aca="false">STDEV(E4:E31)</f>
+        <v>0.0354645162033391</v>
+      </c>
+      <c r="F45" s="4" t="n">
+        <f aca="false">STDEV(F4:F31)</f>
+        <v>0.0331099424739954</v>
+      </c>
+      <c r="G45" s="4" t="n">
+        <f aca="false">STDEV(G4:G31)</f>
+        <v>0.0399718409900924</v>
+      </c>
+      <c r="H45" s="4" t="n">
+        <f aca="false">STDEV(H4:H31)</f>
+        <v>0.0193757411280759</v>
+      </c>
+      <c r="I45" s="4" t="n">
+        <f aca="false">STDEV(I4:I31)</f>
+        <v>0.032748296340906</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <f aca="false">COUNTIF(B4:B31,"&gt;0")</f>
+        <v>9</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <f aca="false">COUNTIF(C4:C31,"&gt;0")</f>
+        <v>12</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <f aca="false">COUNTIF(D4:D31,"&gt;0")</f>
+        <v>8</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <f aca="false">COUNTIF(E4:E31,"&gt;0")</f>
+        <v>11</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <f aca="false">COUNTIF(F4:F31,"&gt;0")</f>
+        <v>9</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <f aca="false">COUNTIF(G4:G31,"&gt;0")</f>
+        <v>9</v>
+      </c>
+      <c r="H46" s="0" t="n">
+        <f aca="false">COUNTIF(H4:H31,"&gt;0")</f>
+        <v>10</v>
+      </c>
+      <c r="I46" s="0" t="n">
+        <f aca="false">COUNTIF(I4:I31,"&gt;0")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <f aca="false">COUNTIF(B4:B31,"&lt;=0")</f>
+        <v>19</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <f aca="false">COUNTIF(C4:C31,"&lt;=0")</f>
+        <v>16</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <f aca="false">COUNTIF(D4:D31,"&lt;=0")</f>
+        <v>20</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <f aca="false">COUNTIF(E4:E31,"&lt;=0")</f>
+        <v>17</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <f aca="false">COUNTIF(F4:F31,"&lt;=0")</f>
+        <v>19</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <f aca="false">COUNTIF(G4:G31,"&lt;=0")</f>
+        <v>19</v>
+      </c>
+      <c r="H47" s="0" t="n">
+        <f aca="false">COUNTIF(H4:H31,"&lt;=0")</f>
+        <v>18</v>
+      </c>
+      <c r="I47" s="0" t="n">
+        <f aca="false">COUNTIF(I4:I31,"&lt;=0")</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48" s="4" t="n">
+        <f aca="false">MAX(B4:B31)</f>
+        <v>0.0233358723</v>
+      </c>
+      <c r="C48" s="4" t="n">
+        <f aca="false">MAX(C4:C31)</f>
+        <v>0.0684339912576881</v>
+      </c>
+      <c r="D48" s="4" t="n">
+        <f aca="false">MAX(D4:D31)</f>
+        <v>0.0230040277518249</v>
+      </c>
+      <c r="E48" s="4" t="n">
+        <f aca="false">MAX(E4:E31)</f>
+        <v>0.0185136</v>
+      </c>
+      <c r="F48" s="4" t="n">
+        <f aca="false">MAX(F4:F31)</f>
+        <v>0.0432471869039501</v>
+      </c>
+      <c r="G48" s="4" t="n">
+        <f aca="false">MAX(G4:G31)</f>
+        <v>0.0952013567694881</v>
+      </c>
+      <c r="H48" s="4" t="n">
+        <f aca="false">MAX(H4:H31)</f>
+        <v>0.02153774981795</v>
+      </c>
+      <c r="I48" s="4" t="n">
+        <f aca="false">MAX(I4:I31)</f>
+        <v>0.0604585318305874</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49" s="4" t="n">
+        <f aca="false">MIN(B4:B31)</f>
+        <v>-0.1123016711</v>
+      </c>
+      <c r="C49" s="4" t="n">
+        <f aca="false">MIN(C4:C31)</f>
+        <v>-0.129376794331987</v>
+      </c>
+      <c r="D49" s="4" t="n">
+        <f aca="false">MIN(D4:D31)</f>
+        <v>-0.0386054491312377</v>
+      </c>
+      <c r="E49" s="4" t="n">
+        <f aca="false">MIN(E4:E31)</f>
+        <v>-0.114673144447425</v>
+      </c>
+      <c r="F49" s="4" t="n">
+        <f aca="false">MIN(F4:F31)</f>
+        <v>-0.128729019240375</v>
+      </c>
+      <c r="G49" s="4" t="n">
+        <f aca="false">MIN(G4:G31)</f>
+        <v>-0.0943216034791614</v>
+      </c>
+      <c r="H49" s="4" t="n">
+        <f aca="false">MIN(H4:H31)</f>
+        <v>-0.0648045595957615</v>
+      </c>
+      <c r="I49" s="4" t="n">
+        <f aca="false">MIN(I4:I31)</f>
         <v>-0.0833472266552495</v>
       </c>
     </row>
@@ -1730,22 +1828,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="71.9234693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3367346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="18.6836734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5255102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="12.5255102040816"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="13.6071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.75"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="73.1122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.7448979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.6887755102041"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="12.7448979591837"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="13.7142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.85714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1781,28 +1879,28 @@
       <c r="A2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="7" t="n">
+      <c r="B2" s="6" t="n">
         <v>2.77555756156289E-017</v>
       </c>
-      <c r="C2" s="7" t="n">
+      <c r="C2" s="6" t="n">
         <v>-0.0106787246939123</v>
       </c>
-      <c r="D2" s="7" t="n">
+      <c r="D2" s="6" t="n">
         <v>-5.55111512312578E-017</v>
       </c>
-      <c r="E2" s="7" t="n">
+      <c r="E2" s="6" t="n">
         <v>0.0304736854104133</v>
       </c>
-      <c r="F2" s="7" t="n">
+      <c r="F2" s="6" t="n">
         <v>-0.00245924135463701</v>
       </c>
-      <c r="G2" s="7" t="n">
+      <c r="G2" s="6" t="n">
         <v>-0.0310530297612995</v>
       </c>
-      <c r="H2" s="7" t="n">
+      <c r="H2" s="6" t="n">
         <v>0.0183998037009875</v>
       </c>
-      <c r="I2" s="7" t="n">
+      <c r="I2" s="6" t="n">
         <v>-0.0332758763385617</v>
       </c>
     </row>
@@ -1810,28 +1908,28 @@
       <c r="A3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="7" t="n">
+      <c r="B3" s="6" t="n">
         <v>0.145344201702701</v>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="C3" s="6" t="n">
         <v>0.144332116031739</v>
       </c>
-      <c r="D3" s="7" t="n">
+      <c r="D3" s="6" t="n">
         <v>0.267001717411063</v>
       </c>
-      <c r="E3" s="7" t="n">
+      <c r="E3" s="6" t="n">
         <v>0.203655817993814</v>
       </c>
-      <c r="F3" s="7" t="n">
+      <c r="F3" s="6" t="n">
         <v>-0.0441788187134618</v>
       </c>
-      <c r="G3" s="7" t="n">
+      <c r="G3" s="6" t="n">
         <v>0.106206779485939</v>
       </c>
-      <c r="H3" s="7" t="n">
+      <c r="H3" s="6" t="n">
         <v>0.118054757995126</v>
       </c>
-      <c r="I3" s="7" t="n">
+      <c r="I3" s="6" t="n">
         <v>-0.00618809530156128</v>
       </c>
     </row>
@@ -1839,28 +1937,28 @@
       <c r="A4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="7" t="n">
+      <c r="B4" s="6" t="n">
         <v>0.00396034478403858</v>
       </c>
-      <c r="C4" s="7" t="n">
+      <c r="C4" s="6" t="n">
         <v>-0.0192502036295736</v>
       </c>
-      <c r="D4" s="7" t="n">
+      <c r="D4" s="6" t="n">
         <v>-0.0721412953841122</v>
       </c>
-      <c r="E4" s="7" t="n">
+      <c r="E4" s="6" t="n">
         <v>-0.112017545365074</v>
       </c>
-      <c r="F4" s="7" t="n">
+      <c r="F4" s="6" t="n">
         <v>-0.110530838197674</v>
       </c>
-      <c r="G4" s="7" t="n">
+      <c r="G4" s="6" t="n">
         <v>0.107683817086788</v>
       </c>
-      <c r="H4" s="7" t="n">
+      <c r="H4" s="6" t="n">
         <v>-0.0597711572392615</v>
       </c>
-      <c r="I4" s="7" t="n">
+      <c r="I4" s="6" t="n">
         <v>-0.0783138242987495</v>
       </c>
     </row>
@@ -1868,28 +1966,28 @@
       <c r="A5" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="7" t="n">
+      <c r="B5" s="6" t="n">
         <v>-0.0272499995889372</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="6" t="n">
         <v>-0.129376794331987</v>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="D5" s="6" t="n">
         <v>-0.0428741646444501</v>
       </c>
-      <c r="E5" s="7" t="n">
+      <c r="E5" s="6" t="n">
         <v>-0.0177288737844371</v>
       </c>
-      <c r="F5" s="7" t="n">
+      <c r="F5" s="6" t="n">
         <v>-0.0719292875692122</v>
       </c>
-      <c r="G5" s="7" t="n">
+      <c r="G5" s="6" t="n">
         <v>-0.0943216034791614</v>
       </c>
-      <c r="H5" s="7" t="n">
+      <c r="H5" s="6" t="n">
         <v>-0.0269998842336498</v>
       </c>
-      <c r="I5" s="7" t="n">
+      <c r="I5" s="6" t="n">
         <v>-0.0723646706184994</v>
       </c>
     </row>
@@ -1897,28 +1995,28 @@
       <c r="A6" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="7" t="n">
+      <c r="B6" s="6" t="n">
         <v>-0.014705266907887</v>
       </c>
-      <c r="C6" s="7" t="n">
+      <c r="C6" s="6" t="n">
         <v>0.0109357638762876</v>
       </c>
-      <c r="D6" s="7" t="n">
+      <c r="D6" s="6" t="n">
         <v>-0.0348606601033247</v>
       </c>
-      <c r="E6" s="7" t="n">
+      <c r="E6" s="6" t="n">
         <v>-0.00875629679457498</v>
       </c>
-      <c r="F6" s="7" t="n">
+      <c r="F6" s="6" t="n">
         <v>-0.0275067718414618</v>
       </c>
-      <c r="G6" s="7" t="n">
+      <c r="G6" s="6" t="n">
         <v>-0.0323798030531991</v>
       </c>
-      <c r="H6" s="7" t="n">
+      <c r="H6" s="6" t="n">
         <v>-0.0054164637098747</v>
       </c>
-      <c r="I6" s="7" t="n">
+      <c r="I6" s="6" t="n">
         <v>-0.0323798030531991</v>
       </c>
     </row>
@@ -1926,28 +2024,28 @@
       <c r="A7" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="7" t="n">
+      <c r="B7" s="6" t="n">
         <v>-0.0247509684356123</v>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="6" t="n">
         <v>0.0429142848892252</v>
       </c>
-      <c r="D7" s="7" t="n">
+      <c r="D7" s="6" t="n">
         <v>0.00713884096551277</v>
       </c>
-      <c r="E7" s="7" t="n">
+      <c r="E7" s="6" t="n">
         <v>0.0155161253507749</v>
       </c>
-      <c r="F7" s="7" t="n">
+      <c r="F7" s="6" t="n">
         <v>-0.0303067468796497</v>
       </c>
-      <c r="G7" s="7" t="n">
+      <c r="G7" s="6" t="n">
         <v>-0.0498064571616875</v>
       </c>
-      <c r="H7" s="7" t="n">
+      <c r="H7" s="6" t="n">
         <v>-0.0188718413918249</v>
       </c>
-      <c r="I7" s="7" t="n">
+      <c r="I7" s="6" t="n">
         <v>0.0748257507764999</v>
       </c>
     </row>
@@ -1955,28 +2053,28 @@
       <c r="A8" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="7" t="n">
+      <c r="B8" s="6" t="n">
         <v>-0.00764560582064955</v>
       </c>
-      <c r="C8" s="7" t="n">
+      <c r="C8" s="6" t="n">
         <v>-0.0524743376033492</v>
       </c>
-      <c r="D8" s="7" t="n">
+      <c r="D8" s="6" t="n">
         <v>-0.00482415509107501</v>
       </c>
-      <c r="E8" s="7" t="n">
+      <c r="E8" s="6" t="n">
         <v>-0.0976869654276871</v>
       </c>
-      <c r="F8" s="7" t="n">
+      <c r="F8" s="6" t="n">
         <v>-0.0299948912120869</v>
       </c>
-      <c r="G8" s="7" t="n">
+      <c r="G8" s="6" t="n">
         <v>-0.0640394522749116</v>
       </c>
-      <c r="H8" s="7" t="n">
+      <c r="H8" s="6" t="n">
         <v>-0.0267274600701122</v>
       </c>
-      <c r="I8" s="7" t="n">
+      <c r="I8" s="6" t="n">
         <v>-0.0290183798169993</v>
       </c>
     </row>
@@ -1984,28 +2082,28 @@
       <c r="A9" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="7" t="n">
+      <c r="B9" s="6" t="n">
         <v>-0.0290415097224873</v>
       </c>
-      <c r="C9" s="7" t="n">
+      <c r="C9" s="6" t="n">
         <v>-0.00735334369044975</v>
       </c>
-      <c r="D9" s="7" t="n">
+      <c r="D9" s="6" t="n">
         <v>-0.0128186896343001</v>
       </c>
-      <c r="E9" s="7" t="n">
+      <c r="E9" s="6" t="n">
         <v>-0.0192062986787121</v>
       </c>
-      <c r="F9" s="7" t="n">
+      <c r="F9" s="6" t="n">
         <v>-0.0136362613134499</v>
       </c>
-      <c r="G9" s="7" t="n">
+      <c r="G9" s="6" t="n">
         <v>-0.0343340559172998</v>
       </c>
-      <c r="H9" s="7" t="n">
+      <c r="H9" s="6" t="n">
         <v>-0.0136202857905001</v>
       </c>
-      <c r="I9" s="7" t="n">
+      <c r="I9" s="6" t="n">
         <v>-0.0200950194207248</v>
       </c>
     </row>
@@ -2013,28 +2111,28 @@
       <c r="A10" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="7" t="n">
+      <c r="B10" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="C10" s="7" t="n">
+      <c r="C10" s="6" t="n">
         <v>-0.0159119978634121</v>
       </c>
-      <c r="D10" s="7" t="n">
+      <c r="D10" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="E10" s="7" t="n">
+      <c r="E10" s="6" t="n">
         <v>-0.0155946808314871</v>
       </c>
-      <c r="F10" s="7" t="n">
+      <c r="F10" s="6" t="n">
         <v>-0.0282302963921122</v>
       </c>
-      <c r="G10" s="7" t="n">
+      <c r="G10" s="6" t="n">
         <v>0.000583196568075078</v>
       </c>
-      <c r="H10" s="7" t="n">
+      <c r="H10" s="6" t="n">
         <v>-0.00983910541349975</v>
       </c>
-      <c r="I10" s="7" t="n">
+      <c r="I10" s="6" t="n">
         <v>-0.0125413115865245</v>
       </c>
     </row>
@@ -2042,28 +2140,28 @@
       <c r="A11" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="7" t="n">
+      <c r="B11" s="6" t="n">
         <v>-0.0712716608887497</v>
       </c>
-      <c r="C11" s="7" t="n">
+      <c r="C11" s="6" t="n">
         <v>0.0684339912576881</v>
       </c>
-      <c r="D11" s="7" t="n">
+      <c r="D11" s="6" t="n">
         <v>-0.0071472582172373</v>
       </c>
-      <c r="E11" s="7" t="n">
+      <c r="E11" s="6" t="n">
         <v>-0.0190667768793243</v>
       </c>
-      <c r="F11" s="7" t="n">
+      <c r="F11" s="6" t="n">
         <v>-0.0201917142902744</v>
       </c>
-      <c r="G11" s="7" t="n">
+      <c r="G11" s="6" t="n">
         <v>0.0494471305072754</v>
       </c>
-      <c r="H11" s="7" t="n">
+      <c r="H11" s="6" t="n">
         <v>0.0175553213680756</v>
       </c>
-      <c r="I11" s="7" t="n">
+      <c r="I11" s="6" t="n">
         <v>0.0491247945233879</v>
       </c>
     </row>
@@ -2071,28 +2169,28 @@
       <c r="A12" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="7" t="n">
+      <c r="B12" s="6" t="n">
         <v>-0.0123012952089374</v>
       </c>
-      <c r="C12" s="7" t="n">
+      <c r="C12" s="6" t="n">
         <v>0.000270659343312718</v>
       </c>
-      <c r="D12" s="7" t="n">
+      <c r="D12" s="6" t="n">
         <v>-0.00156281758811247</v>
       </c>
-      <c r="E12" s="7" t="n">
+      <c r="E12" s="6" t="n">
         <v>-0.0196208738228246</v>
       </c>
-      <c r="F12" s="7" t="n">
+      <c r="F12" s="6" t="n">
         <v>-0.0063546730654869</v>
       </c>
-      <c r="G12" s="7" t="n">
+      <c r="G12" s="6" t="n">
         <v>-0.0403648051559997</v>
       </c>
-      <c r="H12" s="7" t="n">
+      <c r="H12" s="6" t="n">
         <v>-0.00732162454231189</v>
       </c>
-      <c r="I12" s="7" t="n">
+      <c r="I12" s="6" t="n">
         <v>-0.0231103595869244</v>
       </c>
     </row>
@@ -2100,28 +2198,28 @@
       <c r="A13" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="7" t="n">
+      <c r="B13" s="6" t="n">
         <v>-0.0107701211137874</v>
       </c>
-      <c r="C13" s="7" t="n">
+      <c r="C13" s="6" t="n">
         <v>-0.0191944370401876</v>
       </c>
-      <c r="D13" s="7" t="n">
+      <c r="D13" s="6" t="n">
         <v>-0.00820403442296241</v>
       </c>
-      <c r="E13" s="7" t="n">
+      <c r="E13" s="6" t="n">
         <v>-0.0156824014263247</v>
       </c>
-      <c r="F13" s="7" t="n">
+      <c r="F13" s="6" t="n">
         <v>-0.00830723061372407</v>
       </c>
-      <c r="G13" s="7" t="n">
+      <c r="G13" s="6" t="n">
         <v>-0.0131667997765998</v>
       </c>
-      <c r="H13" s="7" t="n">
+      <c r="H13" s="6" t="n">
         <v>-0.00820403442296241</v>
       </c>
-      <c r="I13" s="7" t="n">
+      <c r="I13" s="6" t="n">
         <v>-0.0365686946122619</v>
       </c>
     </row>
@@ -2129,28 +2227,28 @@
       <c r="A14" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="7" t="n">
+      <c r="B14" s="6" t="n">
         <v>0.00552366588675019</v>
       </c>
-      <c r="C14" s="7" t="n">
+      <c r="C14" s="6" t="n">
         <v>0.0127888628195631</v>
       </c>
-      <c r="D14" s="7" t="n">
+      <c r="D14" s="6" t="n">
         <v>-0.0252464653045124</v>
       </c>
-      <c r="E14" s="7" t="n">
+      <c r="E14" s="6" t="n">
         <v>0.0223900923967505</v>
       </c>
-      <c r="F14" s="7" t="n">
+      <c r="F14" s="6" t="n">
         <v>0.0442049567523503</v>
       </c>
-      <c r="G14" s="7" t="n">
+      <c r="G14" s="6" t="n">
         <v>0.0105471170042382</v>
       </c>
-      <c r="H14" s="7" t="n">
+      <c r="H14" s="6" t="n">
         <v>0.00509154007640038</v>
       </c>
-      <c r="I14" s="7" t="n">
+      <c r="I14" s="6" t="n">
         <v>-0.0251747808925245</v>
       </c>
     </row>
@@ -2158,28 +2256,28 @@
       <c r="A15" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="7" t="n">
+      <c r="B15" s="6" t="n">
         <v>-0.00797066250277509</v>
       </c>
-      <c r="C15" s="7" t="n">
+      <c r="C15" s="6" t="n">
         <v>-0.0323626107811994</v>
       </c>
-      <c r="D15" s="7" t="n">
+      <c r="D15" s="6" t="n">
         <v>-0.0126767342159993</v>
       </c>
-      <c r="E15" s="7" t="n">
+      <c r="E15" s="6" t="n">
         <v>0.0111453439751128</v>
       </c>
-      <c r="F15" s="7" t="n">
+      <c r="F15" s="6" t="n">
         <v>-0.0195782257775498</v>
       </c>
-      <c r="G15" s="7" t="n">
+      <c r="G15" s="6" t="n">
         <v>-0.0224364414199241</v>
       </c>
-      <c r="H15" s="7" t="n">
+      <c r="H15" s="6" t="n">
         <v>0.00252729440360004</v>
       </c>
-      <c r="I15" s="7" t="n">
+      <c r="I15" s="6" t="n">
         <v>0.0111453439751128</v>
       </c>
     </row>
@@ -2187,28 +2285,28 @@
       <c r="A16" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="7" t="n">
+      <c r="B16" s="6" t="n">
         <v>4.85722573273506E-017</v>
       </c>
-      <c r="C16" s="7" t="n">
+      <c r="C16" s="6" t="n">
         <v>-4.16333634234434E-017</v>
       </c>
-      <c r="D16" s="7" t="n">
+      <c r="D16" s="6" t="n">
         <v>-0.0286435454543873</v>
       </c>
-      <c r="E16" s="7" t="n">
+      <c r="E16" s="6" t="n">
         <v>9.0205620750794E-017</v>
       </c>
-      <c r="F16" s="7" t="n">
+      <c r="F16" s="6" t="n">
         <v>-0.026261521507025</v>
       </c>
-      <c r="G16" s="7" t="n">
+      <c r="G16" s="6" t="n">
         <v>-0.0211817696922001</v>
       </c>
-      <c r="H16" s="7" t="n">
+      <c r="H16" s="6" t="n">
         <v>-0.0414655456021746</v>
       </c>
-      <c r="I16" s="7" t="n">
+      <c r="I16" s="6" t="n">
         <v>-0.0279804764373248</v>
       </c>
     </row>
@@ -2216,28 +2314,28 @@
       <c r="A17" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="7" t="n">
+      <c r="B17" s="6" t="n">
         <v>-0.00574095685738732</v>
       </c>
-      <c r="C17" s="7" t="n">
+      <c r="C17" s="6" t="n">
         <v>2.08166817117217E-017</v>
       </c>
-      <c r="D17" s="7" t="n">
+      <c r="D17" s="6" t="n">
         <v>-0.00668755288879982</v>
       </c>
-      <c r="E17" s="7" t="n">
+      <c r="E17" s="6" t="n">
         <v>-0.0142623522480373</v>
       </c>
-      <c r="F17" s="7" t="n">
+      <c r="F17" s="6" t="n">
         <v>-0.00249931975322477</v>
       </c>
-      <c r="G17" s="7" t="n">
+      <c r="G17" s="6" t="n">
         <v>6.93889390390723E-017</v>
       </c>
-      <c r="H17" s="7" t="n">
+      <c r="H17" s="6" t="n">
         <v>-0.0164275299645996</v>
       </c>
-      <c r="I17" s="7" t="n">
+      <c r="I17" s="6" t="n">
         <v>3.46944695195361E-017</v>
       </c>
     </row>
@@ -2245,28 +2343,28 @@
       <c r="A18" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="7" t="n">
+      <c r="B18" s="6" t="n">
         <v>-0.0279886786967253</v>
       </c>
-      <c r="C18" s="7" t="n">
+      <c r="C18" s="6" t="n">
         <v>-0.0148213628184004</v>
       </c>
-      <c r="D18" s="7" t="n">
+      <c r="D18" s="6" t="n">
         <v>-0.017436209081675</v>
       </c>
-      <c r="E18" s="7" t="n">
+      <c r="E18" s="6" t="n">
         <v>-0.0208125186722249</v>
       </c>
-      <c r="F18" s="7" t="n">
+      <c r="F18" s="6" t="n">
         <v>-0.0205899581083501</v>
       </c>
-      <c r="G18" s="7" t="n">
+      <c r="G18" s="6" t="n">
         <v>-0.0198413847866</v>
       </c>
-      <c r="H18" s="7" t="n">
+      <c r="H18" s="6" t="n">
         <v>-0.0208125186722249</v>
       </c>
-      <c r="I18" s="7" t="n">
+      <c r="I18" s="6" t="n">
         <v>0.00761761507305009</v>
       </c>
     </row>
@@ -2274,28 +2372,28 @@
       <c r="A19" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="7" t="n">
+      <c r="B19" s="6" t="n">
         <v>-2.08166817117217E-017</v>
       </c>
-      <c r="C19" s="7" t="n">
+      <c r="C19" s="6" t="n">
         <v>-2.08166817117217E-017</v>
       </c>
-      <c r="D19" s="7" t="n">
+      <c r="D19" s="6" t="n">
         <v>2.08166817117217E-017</v>
       </c>
-      <c r="E19" s="7" t="n">
+      <c r="E19" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="F19" s="7" t="n">
+      <c r="F19" s="6" t="n">
         <v>4.16333634234434E-017</v>
       </c>
-      <c r="G19" s="7" t="n">
+      <c r="G19" s="6" t="n">
         <v>-2.08166817117217E-017</v>
       </c>
-      <c r="H19" s="7" t="n">
+      <c r="H19" s="6" t="n">
         <v>2.08166817117217E-017</v>
       </c>
-      <c r="I19" s="7" t="n">
+      <c r="I19" s="6" t="n">
         <v>-6.93889390390723E-018</v>
       </c>
     </row>
@@ -2303,28 +2401,28 @@
       <c r="A20" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="7" t="n">
+      <c r="B20" s="6" t="n">
         <v>-0.0290000402786251</v>
       </c>
-      <c r="C20" s="7" t="n">
+      <c r="C20" s="6" t="n">
         <v>-0.0268362234190621</v>
       </c>
-      <c r="D20" s="7" t="n">
+      <c r="D20" s="6" t="n">
         <v>-0.00438226163049992</v>
       </c>
-      <c r="E20" s="7" t="n">
+      <c r="E20" s="6" t="n">
         <v>-0.0280646060995745</v>
       </c>
-      <c r="F20" s="7" t="n">
+      <c r="F20" s="6" t="n">
         <v>-0.0290000402786251</v>
       </c>
-      <c r="G20" s="7" t="n">
+      <c r="G20" s="6" t="n">
         <v>-0.0215561456171249</v>
       </c>
-      <c r="H20" s="7" t="n">
+      <c r="H20" s="6" t="n">
         <v>-0.00438226163049992</v>
       </c>
-      <c r="I20" s="7" t="n">
+      <c r="I20" s="6" t="n">
         <v>-0.0410828377885252</v>
       </c>
     </row>
@@ -2332,28 +2430,28 @@
       <c r="A21" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="7" t="n">
+      <c r="B21" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="C21" s="7" t="n">
+      <c r="C21" s="6" t="n">
         <v>-0.0332158693464373</v>
       </c>
-      <c r="D21" s="7" t="n">
+      <c r="D21" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="E21" s="7" t="n">
+      <c r="E21" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="F21" s="7" t="n">
+      <c r="F21" s="6" t="n">
         <v>4.16333634234434E-017</v>
       </c>
-      <c r="G21" s="7" t="n">
+      <c r="G21" s="6" t="n">
         <v>2.08166817117217E-017</v>
       </c>
-      <c r="H21" s="7" t="n">
+      <c r="H21" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="I21" s="7" t="n">
+      <c r="I21" s="6" t="n">
         <v>4.16333634234434E-017</v>
       </c>
     </row>
@@ -2361,28 +2459,28 @@
       <c r="A22" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="7" t="n">
+      <c r="B22" s="6" t="n">
         <v>-0.0153089975691874</v>
       </c>
-      <c r="C22" s="7" t="n">
+      <c r="C22" s="6" t="n">
         <v>0.0271727083889379</v>
       </c>
-      <c r="D22" s="7" t="n">
+      <c r="D22" s="6" t="n">
         <v>0.00811304181160019</v>
       </c>
-      <c r="E22" s="7" t="n">
+      <c r="E22" s="6" t="n">
         <v>-0.027972589353387</v>
       </c>
-      <c r="F22" s="7" t="n">
+      <c r="F22" s="6" t="n">
         <v>0.0161992101130753</v>
       </c>
-      <c r="G22" s="7" t="n">
+      <c r="G22" s="6" t="n">
         <v>0.0677799695274879</v>
       </c>
-      <c r="H22" s="7" t="n">
+      <c r="H22" s="6" t="n">
         <v>0.00811304181160019</v>
       </c>
-      <c r="I22" s="7" t="n">
+      <c r="I22" s="6" t="n">
         <v>0.0220331267622504</v>
       </c>
     </row>
@@ -2390,28 +2488,28 @@
       <c r="A23" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="7" t="n">
+      <c r="B23" s="6" t="n">
         <v>-0.010417387004262</v>
       </c>
-      <c r="C23" s="7" t="n">
+      <c r="C23" s="6" t="n">
         <v>-0.0377310351646493</v>
       </c>
-      <c r="D23" s="7" t="n">
+      <c r="D23" s="6" t="n">
         <v>0.00752526242849996</v>
       </c>
-      <c r="E23" s="7" t="n">
+      <c r="E23" s="6" t="n">
         <v>-0.0633291357194241</v>
       </c>
-      <c r="F23" s="7" t="n">
+      <c r="F23" s="6" t="n">
         <v>0.00105001699195029</v>
       </c>
-      <c r="G23" s="7" t="n">
+      <c r="G23" s="6" t="n">
         <v>-0.0787446031843369</v>
       </c>
-      <c r="H23" s="7" t="n">
+      <c r="H23" s="6" t="n">
         <v>0.00752526242849996</v>
       </c>
-      <c r="I23" s="7" t="n">
+      <c r="I23" s="6" t="n">
         <v>-0.0248696412082121</v>
       </c>
     </row>
@@ -2419,28 +2517,28 @@
       <c r="A24" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="7" t="n">
+      <c r="B24" s="6" t="n">
         <v>0.00763968820842517</v>
       </c>
-      <c r="C24" s="7" t="n">
+      <c r="C24" s="6" t="n">
         <v>-0.0340519350862248</v>
       </c>
-      <c r="D24" s="7" t="n">
+      <c r="D24" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="E24" s="7" t="n">
+      <c r="E24" s="6" t="n">
         <v>-0.0298596137213624</v>
       </c>
-      <c r="F24" s="7" t="n">
+      <c r="F24" s="6" t="n">
         <v>-0.00946205553037492</v>
       </c>
-      <c r="G24" s="7" t="n">
+      <c r="G24" s="6" t="n">
         <v>-0.066824139417087</v>
       </c>
-      <c r="H24" s="7" t="n">
+      <c r="H24" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="I24" s="7" t="n">
+      <c r="I24" s="6" t="n">
         <v>-0.0407846092931371</v>
       </c>
     </row>
@@ -2448,28 +2546,28 @@
       <c r="A25" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="7" t="n">
+      <c r="B25" s="6" t="n">
         <v>3.12250225675825E-017</v>
       </c>
-      <c r="C25" s="7" t="n">
+      <c r="C25" s="6" t="n">
         <v>3.12250225675825E-017</v>
       </c>
-      <c r="D25" s="7" t="n">
+      <c r="D25" s="6" t="n">
         <v>3.12250225675825E-017</v>
       </c>
-      <c r="E25" s="7" t="n">
+      <c r="E25" s="6" t="n">
         <v>-0.00629073077864947</v>
       </c>
-      <c r="F25" s="7" t="n">
+      <c r="F25" s="6" t="n">
         <v>6.93889390390723E-018</v>
       </c>
-      <c r="G25" s="7" t="n">
+      <c r="G25" s="6" t="n">
         <v>3.12250225675825E-017</v>
       </c>
-      <c r="H25" s="7" t="n">
+      <c r="H25" s="6" t="n">
         <v>3.12250225675825E-017</v>
       </c>
-      <c r="I25" s="7" t="n">
+      <c r="I25" s="6" t="n">
         <v>-0.0265983461914497</v>
       </c>
     </row>
@@ -2477,28 +2575,28 @@
       <c r="A26" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="7" t="n">
+      <c r="B26" s="6" t="n">
         <v>9.71445146547012E-017</v>
       </c>
-      <c r="C26" s="7" t="n">
+      <c r="C26" s="6" t="n">
         <v>-2.08166817117217E-017</v>
       </c>
-      <c r="D26" s="7" t="n">
+      <c r="D26" s="6" t="n">
         <v>-3.46944695195361E-017</v>
       </c>
-      <c r="E26" s="7" t="n">
+      <c r="E26" s="6" t="n">
         <v>2.08166817117217E-017</v>
       </c>
-      <c r="F26" s="7" t="n">
+      <c r="F26" s="6" t="n">
         <v>9.71445146547012E-017</v>
       </c>
-      <c r="G26" s="7" t="n">
+      <c r="G26" s="6" t="n">
         <v>4.16333634234434E-017</v>
       </c>
-      <c r="H26" s="7" t="n">
+      <c r="H26" s="6" t="n">
         <v>-3.46944695195361E-017</v>
       </c>
-      <c r="I26" s="7" t="n">
+      <c r="I26" s="6" t="n">
         <v>-6.93889390390723E-017</v>
       </c>
     </row>
@@ -2506,28 +2604,28 @@
       <c r="A27" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="7" t="n">
+      <c r="B27" s="6" t="n">
         <v>-1.38777878078145E-017</v>
       </c>
-      <c r="C27" s="7" t="n">
+      <c r="C27" s="6" t="n">
         <v>-9.71445146547012E-017</v>
       </c>
-      <c r="D27" s="7" t="n">
+      <c r="D27" s="6" t="n">
         <v>-9.71445146547012E-017</v>
       </c>
-      <c r="E27" s="7" t="n">
+      <c r="E27" s="6" t="n">
         <v>-6.24500451351651E-017</v>
       </c>
-      <c r="F27" s="7" t="n">
+      <c r="F27" s="6" t="n">
         <v>-1.38777878078145E-017</v>
       </c>
-      <c r="G27" s="7" t="n">
+      <c r="G27" s="6" t="n">
         <v>-9.71445146547012E-017</v>
       </c>
-      <c r="H27" s="7" t="n">
+      <c r="H27" s="6" t="n">
         <v>-9.71445146547012E-017</v>
       </c>
-      <c r="I27" s="7" t="n">
+      <c r="I27" s="6" t="n">
         <v>-9.71445146547012E-017</v>
       </c>
     </row>
@@ -2535,28 +2633,28 @@
       <c r="A28" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="7" t="n">
+      <c r="B28" s="6" t="n">
         <v>-0.0177879798042501</v>
       </c>
-      <c r="C28" s="7" t="n">
+      <c r="C28" s="6" t="n">
         <v>-0.0101689071238</v>
       </c>
-      <c r="D28" s="7" t="n">
+      <c r="D28" s="6" t="n">
         <v>-0.0149735978345997</v>
       </c>
-      <c r="E28" s="7" t="n">
+      <c r="E28" s="6" t="n">
         <v>-0.0133491168603002</v>
       </c>
-      <c r="F28" s="7" t="n">
+      <c r="F28" s="6" t="n">
         <v>-0.0177879798042501</v>
       </c>
-      <c r="G28" s="7" t="n">
+      <c r="G28" s="6" t="n">
         <v>-0.0154108123646747</v>
       </c>
-      <c r="H28" s="7" t="n">
+      <c r="H28" s="6" t="n">
         <v>-0.0149735978345997</v>
       </c>
-      <c r="I28" s="7" t="n">
+      <c r="I28" s="6" t="n">
         <v>-0.0036464302038874</v>
       </c>
     </row>
@@ -2564,28 +2662,28 @@
       <c r="A29" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="7" t="n">
+      <c r="B29" s="6" t="n">
         <v>0.013657365048988</v>
       </c>
-      <c r="C29" s="7" t="n">
+      <c r="C29" s="6" t="n">
         <v>-0.0286883191148127</v>
       </c>
-      <c r="D29" s="7" t="n">
+      <c r="D29" s="6" t="n">
         <v>5.55111512312578E-017</v>
       </c>
-      <c r="E29" s="7" t="n">
+      <c r="E29" s="6" t="n">
         <v>0.00636983562653803</v>
       </c>
-      <c r="F29" s="7" t="n">
+      <c r="F29" s="6" t="n">
         <v>0.0239610198279137</v>
       </c>
-      <c r="G29" s="7" t="n">
+      <c r="G29" s="6" t="n">
         <v>-0.046440727705337</v>
       </c>
-      <c r="H29" s="7" t="n">
+      <c r="H29" s="6" t="n">
         <v>5.55111512312578E-017</v>
       </c>
-      <c r="I29" s="7" t="n">
+      <c r="I29" s="6" t="n">
         <v>-0.0357051142984873</v>
       </c>
     </row>
@@ -2593,28 +2691,28 @@
       <c r="A30" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="7" t="n">
+      <c r="B30" s="6" t="n">
         <v>0.00337859883242544</v>
       </c>
-      <c r="C30" s="7" t="n">
+      <c r="C30" s="6" t="n">
         <v>-0.00539620147110001</v>
       </c>
-      <c r="D30" s="7" t="n">
+      <c r="D30" s="6" t="n">
         <v>0.00337859883242544</v>
       </c>
-      <c r="E30" s="7" t="n">
+      <c r="E30" s="6" t="n">
         <v>0.00503260833852495</v>
       </c>
-      <c r="F30" s="7" t="n">
+      <c r="F30" s="6" t="n">
         <v>0.00337859883242544</v>
       </c>
-      <c r="G30" s="7" t="n">
+      <c r="G30" s="6" t="n">
         <v>0.000313788302025039</v>
       </c>
-      <c r="H30" s="7" t="n">
+      <c r="H30" s="6" t="n">
         <v>0.00337859883242544</v>
       </c>
-      <c r="I30" s="7" t="n">
+      <c r="I30" s="6" t="n">
         <v>0.000313788302025039</v>
       </c>
     </row>
@@ -2622,28 +2720,28 @@
       <c r="A31" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="7" t="n">
+      <c r="B31" s="6" t="n">
         <v>0.0109505399436497</v>
       </c>
-      <c r="C31" s="7" t="n">
+      <c r="C31" s="6" t="n">
         <v>-0.0370035516840748</v>
       </c>
-      <c r="D31" s="7" t="n">
+      <c r="D31" s="6" t="n">
         <v>-0.0191061150368999</v>
       </c>
-      <c r="E31" s="7" t="n">
+      <c r="E31" s="6" t="n">
         <v>-0.0518054366174619</v>
       </c>
-      <c r="F31" s="7" t="n">
+      <c r="F31" s="6" t="n">
         <v>0.0203584588025005</v>
       </c>
-      <c r="G31" s="7" t="n">
+      <c r="G31" s="6" t="n">
         <v>-0.0226129379383748</v>
       </c>
-      <c r="H31" s="7" t="n">
+      <c r="H31" s="6" t="n">
         <v>-0.0191061150368999</v>
       </c>
-      <c r="I31" s="7" t="n">
+      <c r="I31" s="6" t="n">
         <v>0.0443911432176763</v>
       </c>
     </row>
@@ -2681,47 +2779,70 @@
       <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="3"/>
+      <c r="B35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="3" t="n">
+      <c r="B36" s="4" t="n">
         <f aca="false">AVERAGE(B2:B31)</f>
         <v>-0.00404989086644273</v>
       </c>
-      <c r="C36" s="3" t="n">
+      <c r="C36" s="4" t="n">
         <f aca="false">AVERAGE(C2:C31)</f>
         <v>-0.00692224894186262</v>
       </c>
-      <c r="D36" s="3" t="n">
+      <c r="D36" s="4" t="n">
         <f aca="false">AVERAGE(D2:D31)</f>
         <v>-0.00068093650279487</v>
       </c>
-      <c r="E36" s="3" t="n">
+      <c r="E36" s="4" t="n">
         <f aca="false">AVERAGE(E2:E31)</f>
         <v>-0.00955077679963131</v>
       </c>
-      <c r="F36" s="3" t="n">
+      <c r="F36" s="4" t="n">
         <f aca="false">AVERAGE(F2:F31)</f>
         <v>-0.0136551203627472</v>
       </c>
-      <c r="G36" s="3" t="n">
+      <c r="G36" s="4" t="n">
         <f aca="false">AVERAGE(G2:G31)</f>
         <v>-0.011065105674133</v>
       </c>
-      <c r="H36" s="3" t="n">
+      <c r="H36" s="4" t="n">
         <f aca="false">AVERAGE(H2:H31)</f>
         <v>-0.00377646016460938</v>
       </c>
-      <c r="I36" s="3" t="n">
+      <c r="I36" s="4" t="n">
         <f aca="false">AVERAGE(I2:I31)</f>
         <v>-0.0120082236105851</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="5" t="n">
@@ -2758,372 +2879,446 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="3" t="n">
-        <f aca="false">AVERAGE(B2:B31)*4</f>
-        <v>-0.0161995634657709</v>
-      </c>
-      <c r="C38" s="3" t="n">
-        <f aca="false">AVERAGE(C2:C31)*4</f>
-        <v>-0.0276889957674505</v>
-      </c>
-      <c r="D38" s="3" t="n">
-        <f aca="false">AVERAGE(D2:D31)*4</f>
-        <v>-0.00272374601117948</v>
-      </c>
-      <c r="E38" s="3" t="n">
-        <f aca="false">AVERAGE(E2:E31)*4</f>
-        <v>-0.0382031071985252</v>
-      </c>
-      <c r="F38" s="3" t="n">
-        <f aca="false">AVERAGE(F2:F31)*4</f>
-        <v>-0.0546204814509887</v>
-      </c>
-      <c r="G38" s="3" t="n">
-        <f aca="false">AVERAGE(G2:G31)*4</f>
-        <v>-0.0442604226965319</v>
-      </c>
-      <c r="H38" s="3" t="n">
-        <f aca="false">AVERAGE(H2:H31)*4</f>
-        <v>-0.0151058406584375</v>
-      </c>
-      <c r="I38" s="3" t="n">
-        <f aca="false">AVERAGE(I2:I31)*4</f>
-        <v>-0.0480328944423402</v>
+      <c r="B38" s="4" t="n">
+        <f aca="false">STDEV(B2:B31)</f>
+        <v>0.0328296065396974</v>
+      </c>
+      <c r="C38" s="4" t="n">
+        <f aca="false">STDEV(C2:C31)</f>
+        <v>0.0437828985877402</v>
+      </c>
+      <c r="D38" s="4" t="n">
+        <f aca="false">STDEV(D2:D31)</f>
+        <v>0.0533701526647701</v>
+      </c>
+      <c r="E38" s="4" t="n">
+        <f aca="false">STDEV(E2:E31)</f>
+        <v>0.0507524802494147</v>
+      </c>
+      <c r="F38" s="4" t="n">
+        <f aca="false">STDEV(F2:F31)</f>
+        <v>0.0286460952532439</v>
+      </c>
+      <c r="G38" s="4" t="n">
+        <f aca="false">STDEV(G2:G31)</f>
+        <v>0.0463153094473948</v>
+      </c>
+      <c r="H38" s="4" t="n">
+        <f aca="false">STDEV(H2:H31)</f>
+        <v>0.0282583689997181</v>
+      </c>
+      <c r="I38" s="4" t="n">
+        <f aca="false">STDEV(I2:I31)</f>
+        <v>0.0324541181270851</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="6" t="n">
-        <f aca="false">B38*100000</f>
-        <v>-1619.95634657709</v>
-      </c>
-      <c r="C39" s="6" t="n">
-        <f aca="false">C38*100000</f>
-        <v>-2768.89957674505</v>
-      </c>
-      <c r="D39" s="6" t="n">
-        <f aca="false">D38*100000</f>
-        <v>-272.374601117948</v>
-      </c>
-      <c r="E39" s="6" t="n">
-        <f aca="false">E38*100000</f>
-        <v>-3820.31071985252</v>
-      </c>
-      <c r="F39" s="6" t="n">
-        <f aca="false">F38*100000</f>
-        <v>-5462.04814509887</v>
-      </c>
-      <c r="G39" s="6" t="n">
-        <f aca="false">G38*100000</f>
-        <v>-4426.04226965319</v>
-      </c>
-      <c r="H39" s="6" t="n">
-        <f aca="false">H38*100000</f>
-        <v>-1510.58406584375</v>
-      </c>
-      <c r="I39" s="6" t="n">
-        <f aca="false">I38*100000</f>
-        <v>-4803.28944423402</v>
+      <c r="B39" s="0" t="n">
+        <f aca="false">COUNTIF(B2:B31,"&gt;0")</f>
+        <v>11</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <f aca="false">COUNTIF(C2:C31,"&gt;0")</f>
+        <v>9</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <f aca="false">COUNTIF(D2:D31,"&gt;0")</f>
+        <v>8</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <f aca="false">COUNTIF(E2:E31,"&gt;0")</f>
+        <v>9</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <f aca="false">COUNTIF(F2:F31,"&gt;0")</f>
+        <v>10</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <f aca="false">COUNTIF(G2:G31,"&gt;0")</f>
+        <v>11</v>
+      </c>
+      <c r="H39" s="0" t="n">
+        <f aca="false">COUNTIF(H2:H31,"&gt;0")</f>
+        <v>11</v>
+      </c>
+      <c r="I39" s="0" t="n">
+        <f aca="false">COUNTIF(I2:I31,"&gt;0")</f>
+        <v>9</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="2" t="n">
-        <f aca="false">STDEV(B2:B31)*SQRT(4)</f>
-        <v>0.0656592130793948</v>
-      </c>
-      <c r="C40" s="2" t="n">
-        <f aca="false">STDEV(C2:C31)*SQRT(4)</f>
-        <v>0.0875657971754803</v>
-      </c>
-      <c r="D40" s="2" t="n">
-        <f aca="false">STDEV(D2:D31)*SQRT(4)</f>
-        <v>0.10674030532954</v>
-      </c>
-      <c r="E40" s="2" t="n">
-        <f aca="false">STDEV(E2:E31)*SQRT(4)</f>
-        <v>0.101504960498829</v>
-      </c>
-      <c r="F40" s="2" t="n">
-        <f aca="false">STDEV(F2:F31)*SQRT(4)</f>
-        <v>0.0572921905064879</v>
-      </c>
-      <c r="G40" s="2" t="n">
-        <f aca="false">STDEV(G2:G31)*SQRT(4)</f>
-        <v>0.0926306188947896</v>
-      </c>
-      <c r="H40" s="2" t="n">
-        <f aca="false">STDEV(H2:H31)*SQRT(4)</f>
-        <v>0.0565167379994361</v>
-      </c>
-      <c r="I40" s="2" t="n">
-        <f aca="false">STDEV(I2:I31)*SQRT(4)</f>
-        <v>0.0649082362541701</v>
+      <c r="B40" s="0" t="n">
+        <f aca="false">COUNTIF(B2:B31,"&lt;=0")</f>
+        <v>19</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <f aca="false">COUNTIF(C2:C31,"&lt;=0")</f>
+        <v>21</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <f aca="false">COUNTIF(D2:D31,"&lt;=0")</f>
+        <v>22</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <f aca="false">COUNTIF(E2:E31,"&lt;=0")</f>
+        <v>21</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <f aca="false">COUNTIF(F2:F31,"&lt;=0")</f>
+        <v>20</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <f aca="false">COUNTIF(G2:G31,"&lt;=0")</f>
+        <v>19</v>
+      </c>
+      <c r="H40" s="0" t="n">
+        <f aca="false">COUNTIF(H2:H31,"&lt;=0")</f>
+        <v>19</v>
+      </c>
+      <c r="I40" s="0" t="n">
+        <f aca="false">COUNTIF(I2:I31,"&lt;=0")</f>
+        <v>21</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="6" t="n">
-        <f aca="false">B40*100000</f>
-        <v>6565.92130793948</v>
-      </c>
-      <c r="C41" s="6" t="n">
-        <f aca="false">C40*100000</f>
-        <v>8756.57971754803</v>
-      </c>
-      <c r="D41" s="6" t="n">
-        <f aca="false">D40*100000</f>
-        <v>10674.030532954</v>
-      </c>
-      <c r="E41" s="6" t="n">
-        <f aca="false">E40*100000</f>
-        <v>10150.4960498829</v>
-      </c>
-      <c r="F41" s="6" t="n">
-        <f aca="false">F40*100000</f>
-        <v>5729.21905064879</v>
-      </c>
-      <c r="G41" s="6" t="n">
-        <f aca="false">G40*100000</f>
-        <v>9263.06188947896</v>
-      </c>
-      <c r="H41" s="6" t="n">
-        <f aca="false">H40*100000</f>
-        <v>5651.67379994361</v>
-      </c>
-      <c r="I41" s="6" t="n">
-        <f aca="false">I40*100000</f>
-        <v>6490.82362541701</v>
+      <c r="B41" s="4" t="n">
+        <f aca="false">MAX(B2:B31)</f>
+        <v>0.145344201702701</v>
+      </c>
+      <c r="C41" s="4" t="n">
+        <f aca="false">MAX(C2:C31)</f>
+        <v>0.144332116031739</v>
+      </c>
+      <c r="D41" s="4" t="n">
+        <f aca="false">MAX(D2:D31)</f>
+        <v>0.267001717411063</v>
+      </c>
+      <c r="E41" s="4" t="n">
+        <f aca="false">MAX(E2:E31)</f>
+        <v>0.203655817993814</v>
+      </c>
+      <c r="F41" s="4" t="n">
+        <f aca="false">MAX(F2:F31)</f>
+        <v>0.0442049567523503</v>
+      </c>
+      <c r="G41" s="4" t="n">
+        <f aca="false">MAX(G2:G31)</f>
+        <v>0.107683817086788</v>
+      </c>
+      <c r="H41" s="4" t="n">
+        <f aca="false">MAX(H2:H31)</f>
+        <v>0.118054757995126</v>
+      </c>
+      <c r="I41" s="4" t="n">
+        <f aca="false">MAX(I2:I31)</f>
+        <v>0.0748257507764999</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B42" s="6" t="n">
-        <f aca="false">B38/B40</f>
-        <v>-0.246721864396737</v>
-      </c>
-      <c r="C42" s="6" t="n">
-        <f aca="false">C38/C40</f>
-        <v>-0.316207887789364</v>
-      </c>
-      <c r="D42" s="6" t="n">
-        <f aca="false">D38/D40</f>
-        <v>-0.0255175025288754</v>
-      </c>
-      <c r="E42" s="6" t="n">
-        <f aca="false">E38/E40</f>
-        <v>-0.376366898827234</v>
-      </c>
-      <c r="F42" s="6" t="n">
-        <f aca="false">F38/F40</f>
-        <v>-0.953366959233359</v>
-      </c>
-      <c r="G42" s="6" t="n">
-        <f aca="false">G38/G40</f>
-        <v>-0.477816333568959</v>
-      </c>
-      <c r="H42" s="6" t="n">
-        <f aca="false">H38/H40</f>
-        <v>-0.267280830301781</v>
-      </c>
-      <c r="I42" s="6" t="n">
-        <f aca="false">I38/I40</f>
-        <v>-0.740012319149317</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" s="6" t="n">
-        <f aca="false">B42*100000</f>
-        <v>-24672.1864396737</v>
-      </c>
-      <c r="C43" s="6" t="n">
-        <f aca="false">C42*100000</f>
-        <v>-31620.7887789364</v>
-      </c>
-      <c r="D43" s="6" t="n">
-        <f aca="false">D42*100000</f>
-        <v>-2551.75025288754</v>
-      </c>
-      <c r="E43" s="6" t="n">
-        <f aca="false">E42*100000</f>
-        <v>-37636.6898827234</v>
-      </c>
-      <c r="F43" s="6" t="n">
-        <f aca="false">F42*100000</f>
-        <v>-95336.6959233359</v>
-      </c>
-      <c r="G43" s="6" t="n">
-        <f aca="false">G42*100000</f>
-        <v>-47781.6333568959</v>
-      </c>
-      <c r="H43" s="6" t="n">
-        <f aca="false">H42*100000</f>
-        <v>-26728.0830301781</v>
-      </c>
-      <c r="I43" s="6" t="n">
-        <f aca="false">I42*100000</f>
-        <v>-74001.2319149318</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44" s="0" t="n">
-        <f aca="false">COUNTIF(B2:B31,"&gt;0")</f>
-        <v>11</v>
-      </c>
-      <c r="C44" s="0" t="n">
-        <f aca="false">COUNTIF(C2:C31,"&gt;0")</f>
-        <v>9</v>
-      </c>
-      <c r="D44" s="0" t="n">
-        <f aca="false">COUNTIF(D2:D31,"&gt;0")</f>
-        <v>8</v>
-      </c>
-      <c r="E44" s="0" t="n">
-        <f aca="false">COUNTIF(E2:E31,"&gt;0")</f>
-        <v>9</v>
-      </c>
-      <c r="F44" s="0" t="n">
-        <f aca="false">COUNTIF(F2:F31,"&gt;0")</f>
-        <v>10</v>
-      </c>
-      <c r="G44" s="0" t="n">
-        <f aca="false">COUNTIF(G2:G31,"&gt;0")</f>
-        <v>11</v>
-      </c>
-      <c r="H44" s="0" t="n">
-        <f aca="false">COUNTIF(H2:H31,"&gt;0")</f>
-        <v>11</v>
-      </c>
-      <c r="I44" s="0" t="n">
-        <f aca="false">COUNTIF(I2:I31,"&gt;0")</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" s="0" t="n">
-        <f aca="false">COUNTIF(B2:B31,"&lt;=0")</f>
-        <v>19</v>
-      </c>
-      <c r="C45" s="0" t="n">
-        <f aca="false">COUNTIF(C2:C31,"&lt;=0")</f>
-        <v>21</v>
-      </c>
-      <c r="D45" s="0" t="n">
-        <f aca="false">COUNTIF(D2:D31,"&lt;=0")</f>
-        <v>22</v>
-      </c>
-      <c r="E45" s="0" t="n">
-        <f aca="false">COUNTIF(E2:E31,"&lt;=0")</f>
-        <v>21</v>
-      </c>
-      <c r="F45" s="0" t="n">
-        <f aca="false">COUNTIF(F2:F31,"&lt;=0")</f>
-        <v>20</v>
-      </c>
-      <c r="G45" s="0" t="n">
-        <f aca="false">COUNTIF(G2:G31,"&lt;=0")</f>
-        <v>19</v>
-      </c>
-      <c r="H45" s="0" t="n">
-        <f aca="false">COUNTIF(H2:H31,"&lt;=0")</f>
-        <v>19</v>
-      </c>
-      <c r="I45" s="0" t="n">
-        <f aca="false">COUNTIF(I2:I31,"&lt;=0")</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46" s="3" t="n">
-        <f aca="false">MAX(B2:B31)</f>
-        <v>0.145344201702701</v>
-      </c>
-      <c r="C46" s="3" t="n">
-        <f aca="false">MAX(C2:C31)</f>
-        <v>0.144332116031739</v>
-      </c>
-      <c r="D46" s="3" t="n">
-        <f aca="false">MAX(D2:D31)</f>
-        <v>0.267001717411063</v>
-      </c>
-      <c r="E46" s="3" t="n">
-        <f aca="false">MAX(E2:E31)</f>
-        <v>0.203655817993814</v>
-      </c>
-      <c r="F46" s="3" t="n">
-        <f aca="false">MAX(F2:F31)</f>
-        <v>0.0442049567523503</v>
-      </c>
-      <c r="G46" s="3" t="n">
-        <f aca="false">MAX(G2:G31)</f>
-        <v>0.107683817086788</v>
-      </c>
-      <c r="H46" s="3" t="n">
-        <f aca="false">MAX(H2:H31)</f>
-        <v>0.118054757995126</v>
-      </c>
-      <c r="I46" s="3" t="n">
-        <f aca="false">MAX(I2:I31)</f>
-        <v>0.0748257507764999</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B47" s="3" t="n">
+      <c r="B42" s="4" t="n">
         <f aca="false">MIN(B2:B31)</f>
         <v>-0.0712716608887497</v>
       </c>
-      <c r="C47" s="3" t="n">
+      <c r="C42" s="4" t="n">
         <f aca="false">MIN(C2:C31)</f>
         <v>-0.129376794331987</v>
       </c>
-      <c r="D47" s="3" t="n">
+      <c r="D42" s="4" t="n">
         <f aca="false">MIN(D2:D31)</f>
         <v>-0.0721412953841122</v>
       </c>
-      <c r="E47" s="3" t="n">
+      <c r="E42" s="4" t="n">
         <f aca="false">MIN(E2:E31)</f>
         <v>-0.112017545365074</v>
       </c>
-      <c r="F47" s="3" t="n">
+      <c r="F42" s="4" t="n">
         <f aca="false">MIN(F2:F31)</f>
         <v>-0.110530838197674</v>
       </c>
-      <c r="G47" s="3" t="n">
+      <c r="G42" s="4" t="n">
         <f aca="false">MIN(G2:G31)</f>
         <v>-0.0943216034791614</v>
       </c>
-      <c r="H47" s="3" t="n">
+      <c r="H42" s="4" t="n">
         <f aca="false">MIN(H2:H31)</f>
         <v>-0.0597711572392615</v>
       </c>
-      <c r="I47" s="3" t="n">
+      <c r="I42" s="4" t="n">
         <f aca="false">MIN(I2:I31)</f>
+        <v>-0.0783138242987495</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" s="4" t="n">
+        <f aca="false">AVERAGE(B4:B31)</f>
+        <v>-0.00953003313199939</v>
+      </c>
+      <c r="C43" s="4" t="n">
+        <f aca="false">AVERAGE(C4:C31)</f>
+        <v>-0.0121900306997752</v>
+      </c>
+      <c r="D43" s="4" t="n">
+        <f aca="false">AVERAGE(D4:D31)</f>
+        <v>-0.0102653504462468</v>
+      </c>
+      <c r="E43" s="4" t="n">
+        <f aca="false">AVERAGE(E4:E31)</f>
+        <v>-0.0185947431211845</v>
+      </c>
+      <c r="F43" s="4" t="n">
+        <f aca="false">AVERAGE(F4:F31)</f>
+        <v>-0.0129648411005113</v>
+      </c>
+      <c r="G43" s="4" t="n">
+        <f aca="false">AVERAGE(G4:G31)</f>
+        <v>-0.0145395328553082</v>
+      </c>
+      <c r="H43" s="4" t="n">
+        <f aca="false">AVERAGE(H4:H31)</f>
+        <v>-0.00891958452265694</v>
+      </c>
+      <c r="I43" s="4" t="n">
+        <f aca="false">AVERAGE(I4:I31)</f>
+        <v>-0.0114565263099082</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" s="5" t="n">
+        <f aca="false">B43*100000</f>
+        <v>-953.003313199939</v>
+      </c>
+      <c r="C44" s="5" t="n">
+        <f aca="false">C43*100000</f>
+        <v>-1219.00306997752</v>
+      </c>
+      <c r="D44" s="5" t="n">
+        <f aca="false">D43*100000</f>
+        <v>-1026.53504462468</v>
+      </c>
+      <c r="E44" s="5" t="n">
+        <f aca="false">E43*100000</f>
+        <v>-1859.47431211845</v>
+      </c>
+      <c r="F44" s="5" t="n">
+        <f aca="false">F43*100000</f>
+        <v>-1296.48411005113</v>
+      </c>
+      <c r="G44" s="5" t="n">
+        <f aca="false">G43*100000</f>
+        <v>-1453.95328553082</v>
+      </c>
+      <c r="H44" s="5" t="n">
+        <f aca="false">H43*100000</f>
+        <v>-891.958452265694</v>
+      </c>
+      <c r="I44" s="5" t="n">
+        <f aca="false">I43*100000</f>
+        <v>-1145.65263099082</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="4" t="n">
+        <f aca="false">STDEV(B4:B31)</f>
+        <v>0.017298916184612</v>
+      </c>
+      <c r="C45" s="4" t="n">
+        <f aca="false">STDEV(C4:C31)</f>
+        <v>0.0343847206214291</v>
+      </c>
+      <c r="D45" s="4" t="n">
+        <f aca="false">STDEV(D4:D31)</f>
+        <v>0.0176133872166453</v>
+      </c>
+      <c r="E45" s="4" t="n">
+        <f aca="false">STDEV(E4:E31)</f>
+        <v>0.0306409254905792</v>
+      </c>
+      <c r="F45" s="4" t="n">
+        <f aca="false">STDEV(F4:F31)</f>
+        <v>0.0290127551539572</v>
+      </c>
+      <c r="G45" s="4" t="n">
+        <f aca="false">STDEV(G4:G31)</f>
+        <v>0.0420396244257084</v>
+      </c>
+      <c r="H45" s="4" t="n">
+        <f aca="false">STDEV(H4:H31)</f>
+        <v>0.0161958457766129</v>
+      </c>
+      <c r="I45" s="4" t="n">
+        <f aca="false">STDEV(I4:I31)</f>
+        <v>0.0333611630576975</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <f aca="false">COUNTIF(B4:B31,"&gt;0")</f>
+        <v>9</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <f aca="false">COUNTIF(C4:C31,"&gt;0")</f>
+        <v>8</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <f aca="false">COUNTIF(D4:D31,"&gt;0")</f>
+        <v>7</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <f aca="false">COUNTIF(E4:E31,"&gt;0")</f>
+        <v>7</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <f aca="false">COUNTIF(F4:F31,"&gt;0")</f>
+        <v>10</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <f aca="false">COUNTIF(G4:G31,"&gt;0")</f>
+        <v>10</v>
+      </c>
+      <c r="H46" s="0" t="n">
+        <f aca="false">COUNTIF(H4:H31,"&gt;0")</f>
+        <v>9</v>
+      </c>
+      <c r="I46" s="0" t="n">
+        <f aca="false">COUNTIF(I4:I31,"&gt;0")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <f aca="false">COUNTIF(B4:B31,"&lt;=0")</f>
+        <v>19</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <f aca="false">COUNTIF(C4:C31,"&lt;=0")</f>
+        <v>20</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <f aca="false">COUNTIF(D4:D31,"&lt;=0")</f>
+        <v>21</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <f aca="false">COUNTIF(E4:E31,"&lt;=0")</f>
+        <v>21</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <f aca="false">COUNTIF(F4:F31,"&lt;=0")</f>
+        <v>18</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <f aca="false">COUNTIF(G4:G31,"&lt;=0")</f>
+        <v>18</v>
+      </c>
+      <c r="H47" s="0" t="n">
+        <f aca="false">COUNTIF(H4:H31,"&lt;=0")</f>
+        <v>19</v>
+      </c>
+      <c r="I47" s="0" t="n">
+        <f aca="false">COUNTIF(I4:I31,"&lt;=0")</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48" s="4" t="n">
+        <f aca="false">MAX(B4:B31)</f>
+        <v>0.013657365048988</v>
+      </c>
+      <c r="C48" s="4" t="n">
+        <f aca="false">MAX(C4:C31)</f>
+        <v>0.0684339912576881</v>
+      </c>
+      <c r="D48" s="4" t="n">
+        <f aca="false">MAX(D4:D31)</f>
+        <v>0.00811304181160019</v>
+      </c>
+      <c r="E48" s="4" t="n">
+        <f aca="false">MAX(E4:E31)</f>
+        <v>0.0223900923967505</v>
+      </c>
+      <c r="F48" s="4" t="n">
+        <f aca="false">MAX(F4:F31)</f>
+        <v>0.0442049567523503</v>
+      </c>
+      <c r="G48" s="4" t="n">
+        <f aca="false">MAX(G4:G31)</f>
+        <v>0.107683817086788</v>
+      </c>
+      <c r="H48" s="4" t="n">
+        <f aca="false">MAX(H4:H31)</f>
+        <v>0.0175553213680756</v>
+      </c>
+      <c r="I48" s="4" t="n">
+        <f aca="false">MAX(I4:I31)</f>
+        <v>0.0748257507764999</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49" s="4" t="n">
+        <f aca="false">MIN(B4:B31)</f>
+        <v>-0.0712716608887497</v>
+      </c>
+      <c r="C49" s="4" t="n">
+        <f aca="false">MIN(C4:C31)</f>
+        <v>-0.129376794331987</v>
+      </c>
+      <c r="D49" s="4" t="n">
+        <f aca="false">MIN(D4:D31)</f>
+        <v>-0.0721412953841122</v>
+      </c>
+      <c r="E49" s="4" t="n">
+        <f aca="false">MIN(E4:E31)</f>
+        <v>-0.112017545365074</v>
+      </c>
+      <c r="F49" s="4" t="n">
+        <f aca="false">MIN(F4:F31)</f>
+        <v>-0.110530838197674</v>
+      </c>
+      <c r="G49" s="4" t="n">
+        <f aca="false">MIN(G4:G31)</f>
+        <v>-0.0943216034791614</v>
+      </c>
+      <c r="H49" s="4" t="n">
+        <f aca="false">MIN(H4:H31)</f>
+        <v>-0.0597711572392615</v>
+      </c>
+      <c r="I49" s="4" t="n">
+        <f aca="false">MIN(I4:I31)</f>
         <v>-0.0783138242987495</v>
       </c>
     </row>
@@ -3143,22 +3338,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F36" activeCellId="0" sqref="F36"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="71.9234693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3367346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="18.6836734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5255102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="12.5255102040816"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="13.6071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.75"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="73.1122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.7448979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.6887755102041"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="12.7448979591837"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="13.7142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.85714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4094,265 +4289,473 @@
       <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="3"/>
+      <c r="B35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="4" t="s">
-        <v>52</v>
+      <c r="A36" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="B36" s="5" t="n">
-        <f aca="false">SUM(B2:B31)</f>
-        <v>71525.5387355434</v>
-      </c>
-      <c r="C36" s="5" t="n">
-        <f aca="false">SUM(C2:C31)</f>
-        <v>48603.2789436188</v>
-      </c>
-      <c r="D36" s="5" t="n">
-        <f aca="false">SUM(D2:D31)</f>
-        <v>66445.0778375695</v>
-      </c>
-      <c r="E36" s="5" t="n">
-        <f aca="false">SUM(E2:E31)</f>
-        <v>29848.8984266699</v>
-      </c>
-      <c r="F36" s="5" t="n">
-        <f aca="false">SUM(F2:F31)</f>
-        <v>23772.9861160162</v>
-      </c>
-      <c r="G36" s="5" t="n">
-        <f aca="false">SUM(G2:G31)</f>
-        <v>28382.1906925601</v>
-      </c>
-      <c r="H36" s="5" t="n">
-        <f aca="false">SUM(H2:H31)</f>
-        <v>44251.0843369546</v>
-      </c>
-      <c r="I36" s="5" t="n">
-        <f aca="false">SUM(I2:I31)</f>
-        <v>18149.682509695</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B37" s="5" t="n">
         <f aca="false">AVERAGE(B2:B31)</f>
         <v>2384.18462451811</v>
       </c>
-      <c r="C37" s="5" t="n">
+      <c r="C36" s="5" t="n">
         <f aca="false">AVERAGE(C2:C31)</f>
         <v>1620.10929812063</v>
       </c>
-      <c r="D37" s="5" t="n">
+      <c r="D36" s="5" t="n">
         <f aca="false">AVERAGE(D2:D31)</f>
         <v>2214.83592791898</v>
       </c>
-      <c r="E37" s="5" t="n">
+      <c r="E36" s="5" t="n">
         <f aca="false">AVERAGE(E2:E31)</f>
         <v>994.963280889001</v>
       </c>
-      <c r="F37" s="5" t="n">
+      <c r="F36" s="5" t="n">
         <f aca="false">AVERAGE(F2:F31)</f>
         <v>792.432870533874</v>
       </c>
-      <c r="G37" s="5" t="n">
+      <c r="G36" s="5" t="n">
         <f aca="false">AVERAGE(G2:G31)</f>
         <v>946.073023085334</v>
       </c>
-      <c r="H37" s="5" t="n">
+      <c r="H36" s="5" t="n">
         <f aca="false">AVERAGE(H2:H31)</f>
         <v>1475.03614456516</v>
       </c>
-      <c r="I37" s="5" t="n">
+      <c r="I36" s="5" t="n">
         <f aca="false">AVERAGE(I2:I31)</f>
         <v>604.989416989836</v>
       </c>
     </row>
+    <row r="37" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="5" t="n">
+        <f aca="false">STDEV(B2:B31)</f>
+        <v>6656.27000888295</v>
+      </c>
+      <c r="C37" s="5" t="n">
+        <f aca="false">STDEV(C2:C31)</f>
+        <v>6614.6617668422</v>
+      </c>
+      <c r="D37" s="5" t="n">
+        <f aca="false">STDEV(D2:D31)</f>
+        <v>6996.64380426849</v>
+      </c>
+      <c r="E37" s="5" t="n">
+        <f aca="false">STDEV(E2:E31)</f>
+        <v>6717.04596795076</v>
+      </c>
+      <c r="F37" s="5" t="n">
+        <f aca="false">STDEV(F2:F31)</f>
+        <v>7475.2731819457</v>
+      </c>
+      <c r="G37" s="5" t="n">
+        <f aca="false">STDEV(G2:G31)</f>
+        <v>8228.07887606131</v>
+      </c>
+      <c r="H37" s="5" t="n">
+        <f aca="false">STDEV(H2:H31)</f>
+        <v>7867.32637550916</v>
+      </c>
+      <c r="I37" s="5" t="n">
+        <f aca="false">STDEV(I2:I31)</f>
+        <v>8802.12418065692</v>
+      </c>
+    </row>
     <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B38" s="5" t="n">
-        <f aca="false">STDEV(B2:B31)</f>
-        <v>6656.27000888295</v>
-      </c>
-      <c r="C38" s="5" t="n">
-        <f aca="false">STDEV(C2:C31)</f>
-        <v>6614.6617668422</v>
-      </c>
-      <c r="D38" s="5" t="n">
-        <f aca="false">STDEV(D2:D31)</f>
-        <v>6996.64380426849</v>
-      </c>
-      <c r="E38" s="5" t="n">
-        <f aca="false">STDEV(E2:E31)</f>
-        <v>6717.04596795076</v>
-      </c>
-      <c r="F38" s="5" t="n">
-        <f aca="false">STDEV(F2:F31)</f>
-        <v>7475.2731819457</v>
-      </c>
-      <c r="G38" s="5" t="n">
-        <f aca="false">STDEV(G2:G31)</f>
-        <v>8228.07887606131</v>
-      </c>
-      <c r="H38" s="5" t="n">
-        <f aca="false">STDEV(H2:H31)</f>
-        <v>7867.32637550916</v>
-      </c>
-      <c r="I38" s="5" t="n">
-        <f aca="false">STDEV(I2:I31)</f>
-        <v>8802.12418065692</v>
+        <v>43</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <f aca="false">COUNTIF(B2:B31,"&gt;0")</f>
+        <v>20</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <f aca="false">COUNTIF(C2:C31,"&gt;0")</f>
+        <v>21</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <f aca="false">COUNTIF(D2:D31,"&gt;0")</f>
+        <v>19</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <f aca="false">COUNTIF(E2:E31,"&gt;0")</f>
+        <v>19</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <f aca="false">COUNTIF(F2:F31,"&gt;0")</f>
+        <v>19</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <f aca="false">COUNTIF(G2:G31,"&gt;0")</f>
+        <v>20</v>
+      </c>
+      <c r="H38" s="0" t="n">
+        <f aca="false">COUNTIF(H2:H31,"&gt;0")</f>
+        <v>20</v>
+      </c>
+      <c r="I38" s="0" t="n">
+        <f aca="false">COUNTIF(I2:I31,"&gt;0")</f>
+        <v>19</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B39" s="0" t="n">
-        <f aca="false">COUNTIF(B2:B31,"&gt;0")</f>
-        <v>20</v>
+        <f aca="false">COUNTIF(B2:B31,"&lt;=0")</f>
+        <v>10</v>
       </c>
       <c r="C39" s="0" t="n">
-        <f aca="false">COUNTIF(C2:C31,"&gt;0")</f>
-        <v>21</v>
+        <f aca="false">COUNTIF(C2:C31,"&lt;=0")</f>
+        <v>9</v>
       </c>
       <c r="D39" s="0" t="n">
-        <f aca="false">COUNTIF(D2:D31,"&gt;0")</f>
-        <v>19</v>
+        <f aca="false">COUNTIF(D2:D31,"&lt;=0")</f>
+        <v>11</v>
       </c>
       <c r="E39" s="0" t="n">
-        <f aca="false">COUNTIF(E2:E31,"&gt;0")</f>
-        <v>19</v>
+        <f aca="false">COUNTIF(E2:E31,"&lt;=0")</f>
+        <v>11</v>
       </c>
       <c r="F39" s="0" t="n">
-        <f aca="false">COUNTIF(F2:F31,"&gt;0")</f>
-        <v>19</v>
+        <f aca="false">COUNTIF(F2:F31,"&lt;=0")</f>
+        <v>11</v>
       </c>
       <c r="G39" s="0" t="n">
-        <f aca="false">COUNTIF(G2:G31,"&gt;0")</f>
-        <v>20</v>
+        <f aca="false">COUNTIF(G2:G31,"&lt;=0")</f>
+        <v>10</v>
       </c>
       <c r="H39" s="0" t="n">
-        <f aca="false">COUNTIF(H2:H31,"&gt;0")</f>
-        <v>20</v>
+        <f aca="false">COUNTIF(H2:H31,"&lt;=0")</f>
+        <v>10</v>
       </c>
       <c r="I39" s="0" t="n">
-        <f aca="false">COUNTIF(I2:I31,"&gt;0")</f>
-        <v>19</v>
+        <f aca="false">COUNTIF(I2:I31,"&lt;=0")</f>
+        <v>11</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="B40" s="0" t="n">
-        <f aca="false">COUNTIF(B2:B31,"&lt;=0")</f>
-        <v>10</v>
-      </c>
-      <c r="C40" s="0" t="n">
-        <f aca="false">COUNTIF(C2:C31,"&lt;=0")</f>
-        <v>9</v>
-      </c>
-      <c r="D40" s="0" t="n">
-        <f aca="false">COUNTIF(D2:D31,"&lt;=0")</f>
-        <v>11</v>
-      </c>
-      <c r="E40" s="0" t="n">
-        <f aca="false">COUNTIF(E2:E31,"&lt;=0")</f>
-        <v>11</v>
-      </c>
-      <c r="F40" s="0" t="n">
-        <f aca="false">COUNTIF(F2:F31,"&lt;=0")</f>
-        <v>11</v>
-      </c>
-      <c r="G40" s="0" t="n">
-        <f aca="false">COUNTIF(G2:G31,"&lt;=0")</f>
-        <v>10</v>
-      </c>
-      <c r="H40" s="0" t="n">
-        <f aca="false">COUNTIF(H2:H31,"&lt;=0")</f>
-        <v>10</v>
-      </c>
-      <c r="I40" s="0" t="n">
-        <f aca="false">COUNTIF(I2:I31,"&lt;=0")</f>
-        <v>11</v>
+        <v>45</v>
+      </c>
+      <c r="B40" s="5" t="n">
+        <f aca="false">MAX(B2:B31)</f>
+        <v>17247.1701471001</v>
+      </c>
+      <c r="C40" s="5" t="n">
+        <f aca="false">MAX(C2:C31)</f>
+        <v>12764.2969688301</v>
+      </c>
+      <c r="D40" s="5" t="n">
+        <f aca="false">MAX(D2:D31)</f>
+        <v>16400.7522481838</v>
+      </c>
+      <c r="E40" s="5" t="n">
+        <f aca="false">MAX(E2:E31)</f>
+        <v>13657.7017121613</v>
+      </c>
+      <c r="F40" s="5" t="n">
+        <f aca="false">MAX(F2:F31)</f>
+        <v>15012.2416079563</v>
+      </c>
+      <c r="G40" s="5" t="n">
+        <f aca="false">MAX(G2:G31)</f>
+        <v>19151.8633369488</v>
+      </c>
+      <c r="H40" s="5" t="n">
+        <f aca="false">MAX(H2:H31)</f>
+        <v>15338.9847221538</v>
+      </c>
+      <c r="I40" s="5" t="n">
+        <f aca="false">MAX(I2:I31)</f>
+        <v>10359.8286045001</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B41" s="5" t="n">
-        <f aca="false">MAX(B2:B31)</f>
-        <v>17247.1701471001</v>
-      </c>
-      <c r="C41" s="5" t="n">
-        <f aca="false">MAX(C2:C31)</f>
-        <v>12764.2969688301</v>
-      </c>
-      <c r="D41" s="5" t="n">
-        <f aca="false">MAX(D2:D31)</f>
-        <v>16400.7522481838</v>
-      </c>
-      <c r="E41" s="5" t="n">
-        <f aca="false">MAX(E2:E31)</f>
-        <v>13657.7017121613</v>
-      </c>
-      <c r="F41" s="5" t="n">
-        <f aca="false">MAX(F2:F31)</f>
-        <v>15012.2416079563</v>
-      </c>
-      <c r="G41" s="5" t="n">
-        <f aca="false">MAX(G2:G31)</f>
-        <v>19151.8633369488</v>
-      </c>
-      <c r="H41" s="5" t="n">
-        <f aca="false">MAX(H2:H31)</f>
-        <v>15338.9847221538</v>
-      </c>
-      <c r="I41" s="5" t="n">
-        <f aca="false">MAX(I2:I31)</f>
-        <v>10359.8286045001</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B42" s="5" t="n">
         <f aca="false">MIN(B2:B31)</f>
         <v>-14512.5087876937</v>
       </c>
-      <c r="C42" s="5" t="n">
+      <c r="C41" s="5" t="n">
         <f aca="false">MIN(C2:C31)</f>
         <v>-13311.8810443912</v>
       </c>
-      <c r="D42" s="5" t="n">
+      <c r="D41" s="5" t="n">
         <f aca="false">MIN(D2:D31)</f>
         <v>-11183.9199377187</v>
       </c>
-      <c r="E42" s="5" t="n">
+      <c r="E41" s="5" t="n">
         <f aca="false">MIN(E2:E31)</f>
         <v>-13249.9806496087</v>
       </c>
-      <c r="F42" s="5" t="n">
+      <c r="F41" s="5" t="n">
         <f aca="false">MIN(F2:F31)</f>
         <v>-17590.5677236762</v>
       </c>
-      <c r="G42" s="5" t="n">
+      <c r="G41" s="5" t="n">
         <f aca="false">MIN(G2:G31)</f>
         <v>-20961.8907815036</v>
       </c>
-      <c r="H42" s="5" t="n">
+      <c r="H41" s="5" t="n">
         <f aca="false">MIN(H2:H31)</f>
         <v>-21472.5499429262</v>
       </c>
-      <c r="I42" s="5" t="n">
+      <c r="I41" s="5" t="n">
         <f aca="false">MIN(I2:I31)</f>
         <v>-33896.8352725949</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="5" t="n">
+        <f aca="false">AVERAGE(B4:B31)</f>
+        <v>2774.10964421797</v>
+      </c>
+      <c r="C42" s="5" t="n">
+        <f aca="false">AVERAGE(C4:C31)</f>
+        <v>2608.10981046611</v>
+      </c>
+      <c r="D42" s="5" t="n">
+        <f aca="false">AVERAGE(D4:D31)</f>
+        <v>2839.54191346386</v>
+      </c>
+      <c r="E42" s="5" t="n">
+        <f aca="false">AVERAGE(E4:E31)</f>
+        <v>1958.46138568745</v>
+      </c>
+      <c r="F42" s="5" t="n">
+        <f aca="false">AVERAGE(F4:F31)</f>
+        <v>2026.15796234709</v>
+      </c>
+      <c r="G42" s="5" t="n">
+        <f aca="false">AVERAGE(G4:G31)</f>
+        <v>2334.63390416584</v>
+      </c>
+      <c r="H42" s="5" t="n">
+        <f aca="false">AVERAGE(H4:H31)</f>
+        <v>2725.16862741722</v>
+      </c>
+      <c r="I42" s="5" t="n">
+        <f aca="false">AVERAGE(I4:I31)</f>
+        <v>2517.75179952531</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="5" t="n">
+        <f aca="false">STDEV(B4:B31)</f>
+        <v>6615.49662124714</v>
+      </c>
+      <c r="C43" s="5" t="n">
+        <f aca="false">STDEV(C4:C31)</f>
+        <v>5632.11008168205</v>
+      </c>
+      <c r="D43" s="5" t="n">
+        <f aca="false">STDEV(D4:D31)</f>
+        <v>6771.68530087734</v>
+      </c>
+      <c r="E43" s="5" t="n">
+        <f aca="false">STDEV(E4:E31)</f>
+        <v>5831.56895467552</v>
+      </c>
+      <c r="F43" s="5" t="n">
+        <f aca="false">STDEV(F4:F31)</f>
+        <v>6020.861879707</v>
+      </c>
+      <c r="G43" s="5" t="n">
+        <f aca="false">STDEV(G4:G31)</f>
+        <v>6501.71337726351</v>
+      </c>
+      <c r="H43" s="5" t="n">
+        <f aca="false">STDEV(H4:H31)</f>
+        <v>6322.35542990202</v>
+      </c>
+      <c r="I43" s="5" t="n">
+        <f aca="false">STDEV(I4:I31)</f>
+        <v>4678.21194135757</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <f aca="false">COUNTIF(B4:B31,"&gt;0")</f>
+        <v>19</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <f aca="false">COUNTIF(C4:C31,"&gt;0")</f>
+        <v>21</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <f aca="false">COUNTIF(D4:D31,"&gt;0")</f>
+        <v>19</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <f aca="false">COUNTIF(E4:E31,"&gt;0")</f>
+        <v>19</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <f aca="false">COUNTIF(F4:F31,"&gt;0")</f>
+        <v>19</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <f aca="false">COUNTIF(G4:G31,"&gt;0")</f>
+        <v>20</v>
+      </c>
+      <c r="H44" s="0" t="n">
+        <f aca="false">COUNTIF(H4:H31,"&gt;0")</f>
+        <v>20</v>
+      </c>
+      <c r="I44" s="0" t="n">
+        <f aca="false">COUNTIF(I4:I31,"&gt;0")</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <f aca="false">COUNTIF(B4:B31,"&lt;=0")</f>
+        <v>9</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <f aca="false">COUNTIF(C4:C31,"&lt;=0")</f>
+        <v>7</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <f aca="false">COUNTIF(D4:D31,"&lt;=0")</f>
+        <v>9</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <f aca="false">COUNTIF(E4:E31,"&lt;=0")</f>
+        <v>9</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <f aca="false">COUNTIF(F4:F31,"&lt;=0")</f>
+        <v>9</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <f aca="false">COUNTIF(G4:G31,"&lt;=0")</f>
+        <v>8</v>
+      </c>
+      <c r="H45" s="0" t="n">
+        <f aca="false">COUNTIF(H4:H31,"&lt;=0")</f>
+        <v>8</v>
+      </c>
+      <c r="I45" s="0" t="n">
+        <f aca="false">COUNTIF(I4:I31,"&lt;=0")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" s="5" t="n">
+        <f aca="false">MAX(B4:B31)</f>
+        <v>17247.1701471001</v>
+      </c>
+      <c r="C46" s="5" t="n">
+        <f aca="false">MAX(C4:C31)</f>
+        <v>12764.2969688301</v>
+      </c>
+      <c r="D46" s="5" t="n">
+        <f aca="false">MAX(D4:D31)</f>
+        <v>16400.7522481838</v>
+      </c>
+      <c r="E46" s="5" t="n">
+        <f aca="false">MAX(E4:E31)</f>
+        <v>13657.7017121613</v>
+      </c>
+      <c r="F46" s="5" t="n">
+        <f aca="false">MAX(F4:F31)</f>
+        <v>15012.2416079563</v>
+      </c>
+      <c r="G46" s="5" t="n">
+        <f aca="false">MAX(G4:G31)</f>
+        <v>19151.8633369488</v>
+      </c>
+      <c r="H46" s="5" t="n">
+        <f aca="false">MAX(H4:H31)</f>
+        <v>15338.9847221538</v>
+      </c>
+      <c r="I46" s="5" t="n">
+        <f aca="false">MAX(I4:I31)</f>
+        <v>10359.8286045001</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47" s="5" t="n">
+        <f aca="false">MIN(B4:B31)</f>
+        <v>-14512.5087876937</v>
+      </c>
+      <c r="C47" s="5" t="n">
+        <f aca="false">MIN(C4:C31)</f>
+        <v>-11687.5050705675</v>
+      </c>
+      <c r="D47" s="5" t="n">
+        <f aca="false">MIN(D4:D31)</f>
+        <v>-11183.9199377187</v>
+      </c>
+      <c r="E47" s="5" t="n">
+        <f aca="false">MIN(E4:E31)</f>
+        <v>-13249.9806496087</v>
+      </c>
+      <c r="F47" s="5" t="n">
+        <f aca="false">MIN(F4:F31)</f>
+        <v>-10993.0973038387</v>
+      </c>
+      <c r="G47" s="5" t="n">
+        <f aca="false">MIN(G4:G31)</f>
+        <v>-10286.157917425</v>
+      </c>
+      <c r="H47" s="5" t="n">
+        <f aca="false">MIN(H4:H31)</f>
+        <v>-11386.88853543</v>
+      </c>
+      <c r="I47" s="5" t="n">
+        <f aca="false">MIN(I4:I31)</f>
+        <v>-5603.33209023999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>